<commit_message>
Add sample pool group property to metadata template
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52FF35AC-BFD2-A34D-9272-58DE846968A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B73554E5-8F9C-8C4D-A6F6-6A7DDD7E7B87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" activeTab="1" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="17500" activeTab="2" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="102">
   <si>
     <t>Measurement Property</t>
   </si>
@@ -166,9 +166,6 @@
     <t>Sample Cleanup (Peptide)</t>
   </si>
   <si>
-    <t>For labeled analysis, independent samples are not measured, only pools. Therefore we need to indicate which sample are in each pool.</t>
-  </si>
-  <si>
     <t>Some times a sample is fractionated and all 7 fractions are measured.</t>
   </si>
   <si>
@@ -350,6 +347,27 @@
   </si>
   <si>
     <t>https://www.ebi.ac.uk/ols4/ontologies/ms</t>
+  </si>
+  <si>
+    <t>Pooled Sample Group</t>
+  </si>
+  <si>
+    <t>In case of pooled sample measurement, indicate with a sample group number (e.g. 1) for samples that are in the same measurement pool</t>
+  </si>
+  <si>
+    <t>The instrument model that has been used for the measurement</t>
+  </si>
+  <si>
+    <t>Sample Label</t>
+  </si>
+  <si>
+    <t>This is just a visual aid simplify sample navigation. This column gets ignored during measurement registration</t>
+  </si>
+  <si>
+    <t>Sample Pool Group</t>
+  </si>
+  <si>
+    <t>number (e.g. 1, 2, 3)</t>
   </si>
 </sst>
 </file>
@@ -771,146 +789,153 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69E707E-F04E-7B45-8A9B-6BA21F625A45}">
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:S33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2:K3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.83203125" customWidth="1"/>
-    <col min="2" max="2" width="14.6640625" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="18" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="14.83203125" customWidth="1"/>
+    <col min="3" max="3" width="14.6640625" customWidth="1"/>
+    <col min="6" max="6" width="27.5" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.5" customWidth="1"/>
+    <col min="9" max="9" width="19.33203125" customWidth="1"/>
+    <col min="10" max="10" width="16.83203125" customWidth="1"/>
+    <col min="11" max="11" width="20" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.6640625" customWidth="1"/>
+    <col min="16" max="16" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C1" s="6" t="s">
+      <c r="B1" s="6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="E1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="P1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="R1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="Q1" s="6" t="s">
+      <c r="S1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L2" s="4"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L33" s="3"/>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M2" s="4"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="M16" s="1"/>
+    </row>
+    <row r="17" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M17" s="3"/>
+    </row>
+    <row r="18" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M18" s="3"/>
+    </row>
+    <row r="19" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M19" s="3"/>
+    </row>
+    <row r="20" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M20" s="3"/>
+    </row>
+    <row r="21" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M21" s="3"/>
+    </row>
+    <row r="22" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M22" s="3"/>
+    </row>
+    <row r="23" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M23" s="3"/>
+    </row>
+    <row r="24" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M24" s="3"/>
+    </row>
+    <row r="25" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M25" s="3"/>
+    </row>
+    <row r="26" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M26" s="3"/>
+    </row>
+    <row r="27" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M27" s="3"/>
+    </row>
+    <row r="28" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M28" s="3"/>
+    </row>
+    <row r="29" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M29" s="3"/>
+    </row>
+    <row r="30" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M30" s="3"/>
+    </row>
+    <row r="31" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M31" s="3"/>
+    </row>
+    <row r="32" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M32" s="3"/>
+    </row>
+    <row r="33" spans="13:13" x14ac:dyDescent="0.2">
+      <c r="M33" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="L34:L1048576 L2:L15" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="M34:M1048576 M2:M15" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
       <formula1>500</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid volume value" error="Please enter whole number values in microliter  (e.g. 5,20,100,...)" sqref="K1:K1048576" xr:uid="{11D57472-5261-F74E-96F9-7F8E7F7EB4D4}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid volume value" error="Please enter whole number values in microliter  (e.g. 5,20,100,...)" sqref="L1:L1048576" xr:uid="{11D57472-5261-F74E-96F9-7F8E7F7EB4D4}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -923,7 +948,7 @@
           <x14:formula1>
             <xm:f>'Digestion Method - Info'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>I1:I1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -933,10 +958,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2562780D-D33F-7F46-B91E-16516421BB07}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C23" sqref="C23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,43 +995,46 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>21</v>
+        <v>98</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>8</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="C5" s="3" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>22</v>
+        <v>2</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>34</v>
+        <v>97</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
@@ -1017,7 +1045,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1028,7 +1056,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1080,20 +1108,23 @@
         <v>16</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="C14" s="3" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -1101,7 +1132,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
@@ -1109,9 +1140,17 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B18" s="3" t="s">
         <v>17</v>
       </c>
     </row>
@@ -1122,10 +1161,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA9A15C-9427-F34B-B818-4D616E8AFF0A}">
-  <dimension ref="A1:P5"/>
+  <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1141,12 +1180,13 @@
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="24" customWidth="1"/>
     <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17.1640625" customWidth="1"/>
+    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>20</v>
       </c>
@@ -1184,19 +1224,22 @@
         <v>30</v>
       </c>
       <c r="M1" s="6" t="s">
+        <v>100</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="P1" s="6" t="s">
+      <c r="Q1" s="6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>11</v>
       </c>
@@ -1207,7 +1250,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1216,19 +1259,22 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
+        <v>36</v>
+      </c>
+      <c r="J2" t="s">
         <v>37</v>
       </c>
-      <c r="J2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -1236,21 +1282,21 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="J4" s="5"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="D5" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="J4" s="5"/>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
-      <c r="D5" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
   </sheetData>
@@ -1275,7 +1321,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>6</v>
@@ -1283,25 +1329,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B5" s="8"/>
     </row>
@@ -1325,12 +1371,12 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B2" t="e" cm="1">
         <f t="array" ref="B2">SM</f>
@@ -1339,217 +1385,217 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="36" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="44" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add asterix to mandatory fields
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F55D8D0-A037-C142-96D0-246A18FDDA69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D15B798-205F-CB45-9514-42E9853C6A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" activeTab="2" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="3440" yWindow="1260" windowWidth="29540" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
   <si>
     <t>Measurement Property</t>
   </si>
@@ -331,9 +331,6 @@
     <t>Enzyme code</t>
   </si>
   <si>
-    <t>Organisation id</t>
-  </si>
-  <si>
     <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
   </si>
   <si>
@@ -362,6 +359,39 @@
   </si>
   <si>
     <t>number (e.g. 1, 2, 3)</t>
+  </si>
+  <si>
+    <t>QBiC Sample Ids*</t>
+  </si>
+  <si>
+    <t>Organisation id*</t>
+  </si>
+  <si>
+    <t>Facility*</t>
+  </si>
+  <si>
+    <t>Instrument*</t>
+  </si>
+  <si>
+    <t>Cycle/Fraction Name*</t>
+  </si>
+  <si>
+    <t>Digestion Method*</t>
+  </si>
+  <si>
+    <t>Digestion Enzyme*</t>
+  </si>
+  <si>
+    <t>Enrichment Method*</t>
+  </si>
+  <si>
+    <t>Injection Volume (uL)*</t>
+  </si>
+  <si>
+    <t>LC Column*</t>
+  </si>
+  <si>
+    <t>LCMS Method*</t>
   </si>
 </sst>
 </file>
@@ -783,24 +813,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B69E707E-F04E-7B45-8A9B-6BA21F625A45}">
+  <sheetPr>
+    <tabColor rgb="FF0070C0"/>
+  </sheetPr>
   <dimension ref="A1:Q33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="M2" sqref="M2"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="2" width="14.83203125" customWidth="1"/>
-    <col min="3" max="3" width="14.6640625" customWidth="1"/>
-    <col min="6" max="6" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19.33203125" customWidth="1"/>
-    <col min="8" max="8" width="16.83203125" customWidth="1"/>
-    <col min="9" max="9" width="20" customWidth="1"/>
-    <col min="10" max="10" width="18" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="9.33203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.6640625" customWidth="1"/>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" customWidth="1"/>
+    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.33203125" customWidth="1"/>
+    <col min="9" max="9" width="16.83203125" customWidth="1"/>
+    <col min="10" max="10" width="20" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
+    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" customWidth="1"/>
     <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
@@ -808,43 +841,43 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>20</v>
+        <v>99</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>1</v>
+        <v>95</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>97</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>100</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>23</v>
+        <v>102</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>24</v>
+        <v>103</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>25</v>
+        <v>104</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>27</v>
+        <v>106</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>98</v>
+        <v>109</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>30</v>
@@ -860,68 +893,68 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="K16" s="1"/>
-    </row>
-    <row r="17" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K17" s="3"/>
-    </row>
-    <row r="18" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K18" s="3"/>
-    </row>
-    <row r="19" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K19" s="3"/>
-    </row>
-    <row r="20" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K20" s="3"/>
-    </row>
-    <row r="21" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K21" s="3"/>
-    </row>
-    <row r="22" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K22" s="3"/>
-    </row>
-    <row r="23" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K23" s="3"/>
-    </row>
-    <row r="24" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K24" s="3"/>
-    </row>
-    <row r="25" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K25" s="3"/>
-    </row>
-    <row r="26" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K26" s="3"/>
-    </row>
-    <row r="27" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K29" s="3"/>
-    </row>
-    <row r="30" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K32" s="3"/>
-    </row>
-    <row r="33" spans="11:11" x14ac:dyDescent="0.2">
-      <c r="K33" s="3"/>
+      <c r="L16" s="1"/>
+    </row>
+    <row r="17" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L26" s="3"/>
+    </row>
+    <row r="27" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="12:12" x14ac:dyDescent="0.2">
+      <c r="L33" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="K34:K1048576 K2:K15" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="L34:L1048576 L2:L15" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
       <formula1>500</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid volume value" error="Please enter whole number values in microliter  (e.g. 5,20,100,...)" sqref="J1:J1048576" xr:uid="{11D57472-5261-F74E-96F9-7F8E7F7EB4D4}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="K1:K1048576" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -930,11 +963,11 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{2D82C767-3EA1-B24E-9118-9B9604CF2E68}">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{47CF6592-1152-5048-BB41-CEF7E4ACA408}">
           <x14:formula1>
             <xm:f>'Digestion Method - Info'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>G1:G1048576</xm:sqref>
+          <xm:sqref>H1:H1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -947,7 +980,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -981,131 +1014,131 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>21</v>
+        <v>97</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>8</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>1</v>
+        <v>21</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>95</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>23</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>33</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>3</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
       </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C13" s="3" t="s">
-        <v>34</v>
-      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>98</v>
+        <v>29</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>94</v>
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -1149,8 +1182,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA9A15C-9427-F34B-B818-4D616E8AFF0A}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="M3" sqref="M3"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1210,7 +1243,7 @@
         <v>29</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>30</v>
@@ -1236,7 +1269,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1257,7 +1290,7 @@
         <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1268,7 +1301,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1276,13 +1309,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1295,7 +1328,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1347,7 +1380,7 @@
   <dimension ref="A1:B45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Refactor pxp metadata properties
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -8,16 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D15B798-205F-CB45-9514-42E9853C6A52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFE71932-7963-0A45-BC55-3258C5A39BE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3440" yWindow="1260" windowWidth="29540" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="2800" yWindow="1060" windowWidth="29540" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Property information" sheetId="3" r:id="rId2"/>
     <sheet name="Allowed values" sheetId="2" r:id="rId3"/>
     <sheet name="Digestion Method - Info" sheetId="4" r:id="rId4"/>
-    <sheet name="Digestion Enzyme - Info" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,30 +38,8 @@
 </workbook>
 </file>
 
-<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
-  <metadataTypes count="1">
-    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
-  </metadataTypes>
-  <futureMetadata name="XLDAPR" count="1">
-    <bk>
-      <extLst>
-        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
-          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
-        </ext>
-      </extLst>
-    </bk>
-  </futureMetadata>
-  <cellMetadata count="1">
-    <bk>
-      <rc t="1" v="0"/>
-    </bk>
-  </cellMetadata>
-</metadata>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
   <si>
     <t>Measurement Property</t>
   </si>
@@ -196,141 +173,6 @@
     <t>see Digestion Enzyme - Info</t>
   </si>
   <si>
-    <t>BNPS-SKATOLE</t>
-  </si>
-  <si>
-    <t>CASPASE1</t>
-  </si>
-  <si>
-    <t>CASPASE2</t>
-  </si>
-  <si>
-    <t>CASPASE3</t>
-  </si>
-  <si>
-    <t>CASPASE4</t>
-  </si>
-  <si>
-    <t>CASPASE5</t>
-  </si>
-  <si>
-    <t>CASPASE6</t>
-  </si>
-  <si>
-    <t>CASPASE7</t>
-  </si>
-  <si>
-    <t>CASPASE8</t>
-  </si>
-  <si>
-    <t>CASPASE9</t>
-  </si>
-  <si>
-    <t>CASPASE10</t>
-  </si>
-  <si>
-    <t>CNBR</t>
-  </si>
-  <si>
-    <t>ENTEROKINASE</t>
-  </si>
-  <si>
-    <t>GRANZYMEB</t>
-  </si>
-  <si>
-    <t>HYDROXYLAMINE</t>
-  </si>
-  <si>
-    <t>NTCB</t>
-  </si>
-  <si>
-    <t>PEPSIN_LOW_PH</t>
-  </si>
-  <si>
-    <t>PEPSIN_HIGH_PH</t>
-  </si>
-  <si>
-    <t>PROLINE-ENDOPEPTIDASE</t>
-  </si>
-  <si>
-    <t>THERMOLYSIN</t>
-  </si>
-  <si>
-    <t>THROMBIN</t>
-  </si>
-  <si>
-    <t>FORMIC_ACID</t>
-  </si>
-  <si>
-    <t>STAPHYLOCOCCAL_PEPTIDASE_I</t>
-  </si>
-  <si>
-    <t>IODOSOBENZOIC_ACID</t>
-  </si>
-  <si>
-    <t>CLOSTRIPAIN:CLOSTRIDIOPEPTIDASE_B</t>
-  </si>
-  <si>
-    <t>TOBACCO_ETCH_VIRUS_PROTEASE</t>
-  </si>
-  <si>
-    <t>NEUTROPHIL_ELASTASE</t>
-  </si>
-  <si>
-    <t>PROTEINASE_K</t>
-  </si>
-  <si>
-    <t>FACTOR_XA</t>
-  </si>
-  <si>
-    <t>ASP-N_ENDOPEPTIDASE</t>
-  </si>
-  <si>
-    <t>ARG-C_PROTEINASE</t>
-  </si>
-  <si>
-    <t>ASP-N_ENDOPEPTIDASE_AND_N-TERMINAL_GLU</t>
-  </si>
-  <si>
-    <t>TRYPSIN</t>
-  </si>
-  <si>
-    <t>LYSC</t>
-  </si>
-  <si>
-    <t>LYSN</t>
-  </si>
-  <si>
-    <t>GLUTAMYL_ENDOPEPTIDASE</t>
-  </si>
-  <si>
-    <t>PNGASE_F</t>
-  </si>
-  <si>
-    <t>PAPAIN</t>
-  </si>
-  <si>
-    <t>IDEZ</t>
-  </si>
-  <si>
-    <t>IDES</t>
-  </si>
-  <si>
-    <t>IGDE</t>
-  </si>
-  <si>
-    <t>CHYMOTRYPSIN_LOW_SPECIFICITY</t>
-  </si>
-  <si>
-    <t>CHYMOTRYPSIN_HIGH_SPECIFICITY</t>
-  </si>
-  <si>
-    <t>CHYMOTRYPSIN</t>
-  </si>
-  <si>
-    <t>Enzyme code</t>
-  </si>
-  <si>
     <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
   </si>
   <si>
@@ -343,9 +185,6 @@
     <t>https://www.ebi.ac.uk/ols4/ontologies/ms</t>
   </si>
   <si>
-    <t>In case of pooled sample measurement, indicate with a sample group number (e.g. 1) for samples that are in the same measurement pool</t>
-  </si>
-  <si>
     <t>The instrument model that has been used for the measurement</t>
   </si>
   <si>
@@ -392,6 +231,18 @@
   </si>
   <si>
     <t>LCMS Method*</t>
+  </si>
+  <si>
+    <t>Labeling Type</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
   </si>
 </sst>
 </file>
@@ -816,10 +667,10 @@
   <sheetPr>
     <tabColor rgb="FF0070C0"/>
   </sheetPr>
-  <dimension ref="A1:Q33"/>
+  <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -828,133 +679,133 @@
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
     <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
-    <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="21.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.83203125" customWidth="1"/>
+    <col min="9" max="9" width="11.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" customWidth="1"/>
+    <col min="11" max="11" width="16.83203125" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="21" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" customWidth="1"/>
+    <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>99</v>
+        <v>53</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>100</v>
+        <v>54</v>
       </c>
       <c r="E1" s="6" t="s">
-        <v>101</v>
+        <v>55</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>102</v>
+        <v>56</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>104</v>
+        <v>64</v>
       </c>
       <c r="I1" s="6" t="s">
-        <v>105</v>
+        <v>65</v>
       </c>
       <c r="J1" s="6" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="K1" s="6" t="s">
-        <v>107</v>
+        <v>59</v>
       </c>
       <c r="L1" s="6" t="s">
-        <v>108</v>
+        <v>60</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>30</v>
+        <v>62</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q1" s="6" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L2" s="4"/>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
-      <c r="L16" s="1"/>
-    </row>
-    <row r="17" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L17" s="3"/>
-    </row>
-    <row r="18" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L18" s="3"/>
-    </row>
-    <row r="19" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L19" s="3"/>
-    </row>
-    <row r="20" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L20" s="3"/>
-    </row>
-    <row r="21" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L21" s="3"/>
-    </row>
-    <row r="22" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L22" s="3"/>
-    </row>
-    <row r="23" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L23" s="3"/>
-    </row>
-    <row r="24" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L24" s="3"/>
-    </row>
-    <row r="25" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L25" s="3"/>
-    </row>
-    <row r="26" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L26" s="3"/>
-    </row>
-    <row r="27" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L27" s="3"/>
-    </row>
-    <row r="28" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L28" s="3"/>
-    </row>
-    <row r="29" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L29" s="3"/>
-    </row>
-    <row r="30" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L30" s="3"/>
-    </row>
-    <row r="31" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L31" s="3"/>
-    </row>
-    <row r="32" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L32" s="3"/>
-    </row>
-    <row r="33" spans="12:12" x14ac:dyDescent="0.2">
-      <c r="L33" s="3"/>
+        <v>66</v>
+      </c>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N2" s="4"/>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="N16" s="1"/>
+    </row>
+    <row r="17" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N17" s="3"/>
+    </row>
+    <row r="18" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N18" s="3"/>
+    </row>
+    <row r="19" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N19" s="3"/>
+    </row>
+    <row r="20" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N20" s="3"/>
+    </row>
+    <row r="21" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N21" s="3"/>
+    </row>
+    <row r="22" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N22" s="3"/>
+    </row>
+    <row r="23" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N23" s="3"/>
+    </row>
+    <row r="24" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N24" s="3"/>
+    </row>
+    <row r="25" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N25" s="3"/>
+    </row>
+    <row r="26" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N26" s="3"/>
+    </row>
+    <row r="27" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N27" s="3"/>
+    </row>
+    <row r="28" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N28" s="3"/>
+    </row>
+    <row r="29" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N29" s="3"/>
+    </row>
+    <row r="30" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N30" s="3"/>
+    </row>
+    <row r="31" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N31" s="3"/>
+    </row>
+    <row r="32" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N32" s="3"/>
+    </row>
+    <row r="33" spans="14:14" x14ac:dyDescent="0.2">
+      <c r="N33" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="L34:L1048576 L2:L15" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
+    <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="N34:N1048576 N2:N15" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
       <formula1>500</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="K1:K1048576" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="M1:M1048576" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -967,7 +818,7 @@
           <x14:formula1>
             <xm:f>'Digestion Method - Info'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>J1:J1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -980,7 +831,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1014,24 +865,24 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>95</v>
+        <v>49</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>96</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>93</v>
+        <v>67</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1064,7 +915,7 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>94</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
@@ -1243,7 +1094,7 @@
         <v>29</v>
       </c>
       <c r="M1" s="6" t="s">
-        <v>97</v>
+        <v>51</v>
       </c>
       <c r="N1" s="6" t="s">
         <v>30</v>
@@ -1269,7 +1120,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>89</v>
+        <v>44</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1290,7 +1141,7 @@
         <v>36</v>
       </c>
       <c r="M2" t="s">
-        <v>98</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1301,7 +1152,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>90</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1309,13 +1160,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>91</v>
+        <v>46</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" s="3" t="s">
-        <v>92</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1373,251 +1224,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AC23FEBF-A01A-EA46-8CE4-A566FF3483FE}">
-  <dimension ref="A1:B45"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" t="e" cm="1">
-        <f t="array" ref="B2">SM</f>
-        <v>#NAME?</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A14" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A16" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" t="s">
-        <v>87</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
Allow freetext for sample pool group to allow more flexibility
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19C12299-806E-B847-A07B-D9FBDB88EAA3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5028A2-0C5E-E743-8CDC-F6EF5EA279D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2800" yWindow="1060" windowWidth="29540" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
@@ -670,7 +670,7 @@
   <dimension ref="A1:R33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
change order of measurement columns as requested
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5028A2-0C5E-E743-8CDC-F6EF5EA279D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972F6ECF-415E-4D44-8684-5945CA017916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="1060" windowWidth="29540" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="33160" yWindow="1780" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Measurement Property</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Ideally the facilites name within the organisation (groupname, etc.)</t>
   </si>
   <si>
-    <t>Index used for multiplexing</t>
-  </si>
-  <si>
     <t>QBiC Sample IDs</t>
   </si>
   <si>
@@ -212,18 +209,12 @@
     <t>Instrument*</t>
   </si>
   <si>
-    <t>Cycle/Fraction Name*</t>
-  </si>
-  <si>
     <t>Digestion Method*</t>
   </si>
   <si>
     <t>Digestion Enzyme*</t>
   </si>
   <si>
-    <t>Enrichment Method*</t>
-  </si>
-  <si>
     <t>Injection Volume (uL)*</t>
   </si>
   <si>
@@ -243,6 +234,9 @@
   </si>
   <si>
     <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
+  </si>
+  <si>
+    <t>the method leading to multiple  cycles or fractions (see Cycle/Fraction Name)</t>
   </si>
 </sst>
 </file>
@@ -669,8 +663,8 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,67 +672,67 @@
     <col min="1" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="M1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -805,7 +799,7 @@
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="L34:L1048576 L2:L15 M10" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
       <formula1>500</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="K1:K1048576" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="N1" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -818,7 +812,7 @@
           <x14:formula1>
             <xm:f>'Digestion Method - Info'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -830,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2562780D-D33F-7F46-B91E-16516421BB07}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,7 +848,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -865,29 +859,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -915,34 +909,34 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -953,18 +947,18 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
@@ -975,7 +969,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
@@ -983,18 +977,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -1002,7 +996,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
@@ -1010,7 +1004,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
@@ -1058,10 +1052,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1070,40 +1064,40 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>4</v>
@@ -1120,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1129,19 +1123,19 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1152,7 +1146,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1160,13 +1154,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1185,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>6</v>
@@ -1199,25 +1193,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8"/>
     </row>

</xml_diff>

<commit_message>
Adjust proteomics columns in sheet and UI (#535)
* fix typo, make fractionation/enrichment optional

* change order of measurement columns as requested
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10211"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A5028A2-0C5E-E743-8CDC-F6EF5EA279D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972F6ECF-415E-4D44-8684-5945CA017916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2800" yWindow="1060" windowWidth="29540" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="33160" yWindow="1780" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Measurement Property</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Ideally the facilites name within the organisation (groupname, etc.)</t>
   </si>
   <si>
-    <t>Index used for multiplexing</t>
-  </si>
-  <si>
     <t>QBiC Sample IDs</t>
   </si>
   <si>
@@ -212,18 +209,12 @@
     <t>Instrument*</t>
   </si>
   <si>
-    <t>Cycle/Fraction Name*</t>
-  </si>
-  <si>
     <t>Digestion Method*</t>
   </si>
   <si>
     <t>Digestion Enzyme*</t>
   </si>
   <si>
-    <t>Enrichment Method*</t>
-  </si>
-  <si>
     <t>Injection Volume (uL)*</t>
   </si>
   <si>
@@ -243,6 +234,9 @@
   </si>
   <si>
     <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
+  </si>
+  <si>
+    <t>the method leading to multiple  cycles or fractions (see Cycle/Fraction Name)</t>
   </si>
 </sst>
 </file>
@@ -669,8 +663,8 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,67 +672,67 @@
     <col min="1" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B1" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="H1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="M1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="I1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="J1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>66</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -805,7 +799,7 @@
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="L34:L1048576 L2:L15 M10" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
       <formula1>500</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="K1:K1048576" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="N1" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -818,7 +812,7 @@
           <x14:formula1>
             <xm:f>'Digestion Method - Info'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -830,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2562780D-D33F-7F46-B91E-16516421BB07}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,7 +848,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -865,29 +859,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -915,34 +909,34 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -953,18 +947,18 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
@@ -975,7 +969,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
@@ -983,18 +977,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -1002,7 +996,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
@@ -1010,7 +1004,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
@@ -1058,10 +1052,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1070,40 +1064,40 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>4</v>
@@ -1120,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1129,19 +1123,19 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1152,7 +1146,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1160,13 +1154,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1185,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>6</v>
@@ -1199,25 +1193,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8"/>
     </row>

</xml_diff>

<commit_message>
use new ptx sheet
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCAE7130-A3DB-DC48-B3F3-7B500C15A26F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972F6ECF-415E-4D44-8684-5945CA017916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="33160" yWindow="1780" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="66">
   <si>
     <t>Measurement Property</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Ideally the facilites name within the organisation (groupname, etc.)</t>
   </si>
   <si>
-    <t>Index used for multiplexing</t>
-  </si>
-  <si>
     <t>QBiC Sample IDs</t>
   </si>
   <si>
@@ -200,6 +197,9 @@
     <t>number (e.g. 1, 2, 3)</t>
   </si>
   <si>
+    <t>QBiC Sample Ids*</t>
+  </si>
+  <si>
     <t>Organisation id*</t>
   </si>
   <si>
@@ -209,18 +209,12 @@
     <t>Instrument*</t>
   </si>
   <si>
-    <t>Cycle/Fraction Name*</t>
-  </si>
-  <si>
     <t>Digestion Method*</t>
   </si>
   <si>
     <t>Digestion Enzyme*</t>
   </si>
   <si>
-    <t>Enrichment Method*</t>
-  </si>
-  <si>
     <t>Injection Volume (uL)*</t>
   </si>
   <si>
@@ -242,7 +236,7 @@
     <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
   </si>
   <si>
-    <t>QBiC Sample Id*</t>
+    <t>the method leading to multiple  cycles or fractions (see Cycle/Fraction Name)</t>
   </si>
 </sst>
 </file>
@@ -669,8 +663,8 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -678,28 +672,28 @@
     <col min="1" max="2" width="14.83203125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
     <col min="4" max="4" width="14.6640625" customWidth="1"/>
-    <col min="7" max="7" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.33203125" customWidth="1"/>
-    <col min="9" max="9" width="16.83203125" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.33203125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="20" customWidth="1"/>
-    <col min="11" max="11" width="21" customWidth="1"/>
-    <col min="12" max="12" width="15.1640625" customWidth="1"/>
+    <col min="11" max="11" width="16" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19" customWidth="1"/>
     <col min="13" max="13" width="16.6640625" customWidth="1"/>
-    <col min="14" max="14" width="15.83203125" customWidth="1"/>
-    <col min="15" max="15" width="11.6640625" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="20.83203125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="21.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>67</v>
+        <v>52</v>
       </c>
       <c r="B1" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C1" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>53</v>
@@ -708,37 +702,37 @@
         <v>54</v>
       </c>
       <c r="F1" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>55</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="I1" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="J1" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="K1" s="6" t="s">
         <v>56</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="M1" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>58</v>
       </c>
-      <c r="J1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="K1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>60</v>
       </c>
-      <c r="L1" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="M1" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="O1" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>65</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -805,7 +799,7 @@
     <dataValidation type="textLength" operator="lessThan" allowBlank="1" showErrorMessage="1" errorTitle="Input too long" error="Currently not more than 500 characters are allowed for a measurement note." promptTitle="Comment your measurement" prompt="Test" sqref="L34:L1048576 L2:L15 M10" xr:uid="{AFB4D5E3-901B-6643-98CF-90174DF75584}">
       <formula1>500</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="K1:K1048576" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid number value" error="Please provide a value &gt; 0" sqref="N1" xr:uid="{13C6D493-ADE8-3949-9E16-00A78201A208}">
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
@@ -818,7 +812,7 @@
           <x14:formula1>
             <xm:f>'Digestion Method - Info'!$A$2:$A$5</xm:f>
           </x14:formula1>
-          <xm:sqref>H1:H1048576</xm:sqref>
+          <xm:sqref>K2:K1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -830,8 +824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2562780D-D33F-7F46-B91E-16516421BB07}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -854,7 +848,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>16</v>
@@ -865,29 +859,29 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>16</v>
@@ -915,34 +909,34 @@
         <v>16</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>16</v>
@@ -953,18 +947,18 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>16</v>
@@ -975,7 +969,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>16</v>
@@ -983,18 +977,18 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -1002,7 +996,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
@@ -1010,7 +1004,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>17</v>
@@ -1058,10 +1052,10 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>20</v>
-      </c>
-      <c r="B1" s="6" t="s">
-        <v>21</v>
       </c>
       <c r="C1" s="6" t="s">
         <v>1</v>
@@ -1070,40 +1064,40 @@
         <v>2</v>
       </c>
       <c r="E1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="F1" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="H1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="K1" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="K1" s="6" t="s">
+      <c r="L1" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="M1" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="M1" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="N1" s="6" t="s">
+      <c r="O1" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="O1" s="6" t="s">
+      <c r="P1" s="6" t="s">
         <v>31</v>
-      </c>
-      <c r="P1" s="6" t="s">
-        <v>32</v>
       </c>
       <c r="Q1" s="6" t="s">
         <v>4</v>
@@ -1120,7 +1114,7 @@
         <v>10</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -1129,19 +1123,19 @@
         <v>10</v>
       </c>
       <c r="G2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="H2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="I2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
-        <v>36</v>
-      </c>
       <c r="M2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.2">
@@ -1152,7 +1146,7 @@
         <v>14</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.2">
@@ -1160,13 +1154,13 @@
         <v>13</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="5"/>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.2">
       <c r="D5" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1191,7 +1185,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>6</v>
@@ -1199,25 +1193,25 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B2" s="8"/>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B3" s="8"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="8" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B4" s="8"/>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="8"/>
     </row>

</xml_diff>

<commit_message>
Enable editing of proteomics measurements (#518)
* Provide Excel File Format support

* Save work

* Save

* Save

* Save progress

* Save

* Implement update

* Fix tests

* Provide missing switch statement

* Fix merge

* Save current status

* Call update service

* Fix tests

* use new ptx sheet

* Address change request

* Address change requests

* Accept suggestion

* Accept suggestion

* Remove SUCCESSFUL enum from error code

* Address change requests

* Optimise imports

* Remove mandatory property check

* fix template header

* fix plural

* Remove size output

* Fix enum

* Fix tests

---------

Co-authored-by: wow-such-code <andreas.friedrich@uni-tuebingen.de>
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{972F6ECF-415E-4D44-8684-5945CA017916}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79B2B2D5-CCEA-3341-BF10-B5525186D350}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33160" yWindow="1780" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
+    <workbookView xWindow="33160" yWindow="1780" windowWidth="28800" windowHeight="17500" xr2:uid="{D4F19D33-EE39-EF46-8DDD-2818EAD74D6D}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -197,46 +197,46 @@
     <t>number (e.g. 1, 2, 3)</t>
   </si>
   <si>
+    <t>Organisation id*</t>
+  </si>
+  <si>
+    <t>Facility*</t>
+  </si>
+  <si>
+    <t>Instrument*</t>
+  </si>
+  <si>
+    <t>Digestion Method*</t>
+  </si>
+  <si>
+    <t>Digestion Enzyme*</t>
+  </si>
+  <si>
+    <t>Injection Volume (uL)*</t>
+  </si>
+  <si>
+    <t>LC Column*</t>
+  </si>
+  <si>
+    <t>LCMS Method*</t>
+  </si>
+  <si>
+    <t>Labeling Type</t>
+  </si>
+  <si>
+    <t>Label</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
+  </si>
+  <si>
+    <t>the method leading to multiple  cycles or fractions (see Cycle/Fraction Name)</t>
+  </si>
+  <si>
     <t>QBiC Sample Ids*</t>
-  </si>
-  <si>
-    <t>Organisation id*</t>
-  </si>
-  <si>
-    <t>Facility*</t>
-  </si>
-  <si>
-    <t>Instrument*</t>
-  </si>
-  <si>
-    <t>Digestion Method*</t>
-  </si>
-  <si>
-    <t>Digestion Enzyme*</t>
-  </si>
-  <si>
-    <t>Injection Volume (uL)*</t>
-  </si>
-  <si>
-    <t>LC Column*</t>
-  </si>
-  <si>
-    <t>LCMS Method*</t>
-  </si>
-  <si>
-    <t>Labeling Type</t>
-  </si>
-  <si>
-    <t>Label</t>
-  </si>
-  <si>
-    <t>Comment</t>
-  </si>
-  <si>
-    <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
-  </si>
-  <si>
-    <t>the method leading to multiple  cycles or fractions (see Cycle/Fraction Name)</t>
   </si>
 </sst>
 </file>
@@ -663,8 +663,8 @@
   </sheetPr>
   <dimension ref="A1:R33"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -687,7 +687,7 @@
   <sheetData>
     <row r="1" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
-        <v>52</v>
+        <v>65</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>48</v>
@@ -696,43 +696,43 @@
         <v>50</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="F1" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G1" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="F1" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>55</v>
-      </c>
       <c r="H1" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I1" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="J1" s="6" t="s">
         <v>22</v>
       </c>
       <c r="K1" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="L1" s="6" t="s">
         <v>56</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>57</v>
       </c>
       <c r="M1" s="6" t="s">
         <v>25</v>
       </c>
       <c r="N1" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="O1" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="P1" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="Q1" s="6"/>
       <c r="R1" s="6"/>
@@ -824,7 +824,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2562780D-D33F-7F46-B91E-16516421BB07}">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -876,7 +876,7 @@
         <v>17</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -953,7 +953,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -1027,7 +1027,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CA9A15C-9427-F34B-B818-4D616E8AFF0A}">
   <dimension ref="A1:Q5"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
fix typos in digestion method preselection
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124864F-3DCA-2740-A285-737260ED93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26080" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="1" r:id="rId4"/>
-    <sheet name="Property information" sheetId="2" r:id="rId5"/>
-    <sheet name="Allowed values" sheetId="3" r:id="rId6"/>
+    <sheet name="Metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Property information" sheetId="2" r:id="rId2"/>
+    <sheet name="Allowed values" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -171,34 +180,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
@@ -207,12 +204,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -284,59 +283,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,25 +310,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa7a7a7"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA7A7A7"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -565,7 +590,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -583,7 +608,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -612,7 +637,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -637,7 +662,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -662,7 +687,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -687,7 +712,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -712,7 +737,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -737,7 +762,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -762,7 +787,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -787,7 +812,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +837,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,9 +850,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -844,7 +875,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -862,7 +893,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -887,7 +918,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,7 +943,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -937,7 +968,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -962,7 +993,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -987,7 +1018,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1043,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1037,7 +1068,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,7 +1093,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1087,7 +1118,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1100,9 +1131,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1116,7 +1153,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1134,7 +1171,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1163,7 +1200,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1188,7 +1225,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1213,7 +1250,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1238,7 +1275,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,7 +1300,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1288,7 +1325,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1313,7 +1350,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1338,7 +1375,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1363,7 +1400,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1376,92 +1413,101 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K2:K33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.8516" style="1" customWidth="1"/>
+    <col min="1" max="2" width="14.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6719" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.3047" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="20" style="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6719" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.8516" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.8516" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="16" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1479,7 +1525,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
+    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1497,7 +1543,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1515,7 +1561,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1533,7 +1579,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1551,7 +1597,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1569,7 +1615,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1587,7 +1633,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1605,7 +1651,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1623,7 +1669,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" ht="17" customHeight="1">
+    <row r="11" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1641,7 +1687,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" ht="17" customHeight="1">
+    <row r="12" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1659,7 +1705,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" ht="17" customHeight="1">
+    <row r="13" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1677,7 +1723,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" ht="17" customHeight="1">
+    <row r="14" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1695,7 +1741,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" ht="17" customHeight="1">
+    <row r="15" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1713,7 +1759,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" ht="17" customHeight="1">
+    <row r="16" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1731,7 +1777,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" ht="17" customHeight="1">
+    <row r="17" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1749,7 +1795,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" ht="17" customHeight="1">
+    <row r="18" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1767,7 +1813,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" ht="17" customHeight="1">
+    <row r="19" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1785,7 +1831,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" ht="17" customHeight="1">
+    <row r="20" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1803,7 +1849,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" ht="17" customHeight="1">
+    <row r="21" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1821,7 +1867,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" ht="17" customHeight="1">
+    <row r="22" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1839,7 +1885,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" ht="17" customHeight="1">
+    <row r="23" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1857,7 +1903,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" ht="17" customHeight="1">
+    <row r="24" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1875,7 +1921,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" ht="17" customHeight="1">
+    <row r="25" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1893,7 +1939,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" ht="17" customHeight="1">
+    <row r="26" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1911,7 +1957,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" ht="17" customHeight="1">
+    <row r="27" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1929,7 +1975,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" ht="17" customHeight="1">
+    <row r="28" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1947,7 +1993,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" ht="17" customHeight="1">
+    <row r="29" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1965,7 +2011,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" ht="17" customHeight="1">
+    <row r="30" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1983,7 +2029,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" ht="17" customHeight="1">
+    <row r="31" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2001,7 +2047,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" ht="17" customHeight="1">
+    <row r="32" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2019,7 +2065,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" ht="17" customHeight="1">
+    <row r="33" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2039,12 +2085,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K33">
-      <formula1>"in gel,in solition,iST poteomics kit,on beads"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K33" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"in gel,in solution,iST proteomics kit,on beads"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2052,200 +2098,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.1719" style="9" customWidth="1"/>
-    <col min="3" max="3" width="86.1719" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="10.8516" style="9" customWidth="1"/>
+    <col min="1" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="86.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="10">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s" s="10">
+      <c r="B1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s" s="10">
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="11">
+    <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s" s="11">
+      <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s" s="11">
+      <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="11">
+    <row r="3" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="11">
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="11">
+    <row r="4" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="11">
+    <row r="5" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="11">
+    <row r="6" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s" s="11">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" t="s" s="11">
+    <row r="7" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="11">
+    <row r="8" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s" s="11">
+      <c r="C8" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="11">
+    <row r="9" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="11">
+      <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" t="s" s="11">
+    <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s" s="11">
+      <c r="B10" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="11">
+    <row r="11" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="11">
+      <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s" s="11">
+      <c r="C11" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" t="s" s="11">
+    <row r="12" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s" s="11">
+      <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s" s="11">
+      <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" t="s" s="11">
+    <row r="13" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s" s="11">
+      <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C13" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" t="s" s="11">
+    <row r="14" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s" s="11">
+      <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" t="s" s="11">
+    <row r="15" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s" s="11">
+      <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="C15" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" t="s" s="11">
+    <row r="16" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s" s="11">
+      <c r="B16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="C16" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" ht="17" customHeight="1">
-      <c r="A17" t="s" s="11">
+    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s" s="11">
+      <c r="B17" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2253,136 +2300,137 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.3516" style="12" customWidth="1"/>
-    <col min="2" max="4" width="16" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.6719" style="12" customWidth="1"/>
-    <col min="6" max="7" width="34.5" style="12" customWidth="1"/>
-    <col min="8" max="9" width="17.3516" style="12" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="12" customWidth="1"/>
-    <col min="11" max="11" width="26.1719" style="12" customWidth="1"/>
-    <col min="12" max="12" width="22.8516" style="12" customWidth="1"/>
-    <col min="13" max="13" width="17" style="12" customWidth="1"/>
-    <col min="14" max="14" width="24" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.8516" style="12" customWidth="1"/>
-    <col min="16" max="16" width="12.1719" style="12" customWidth="1"/>
-    <col min="17" max="16384" width="10.8516" style="12" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="16" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="34.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="17.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="13">
+    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s" s="13">
+      <c r="B2" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" t="s" s="14">
+      <c r="D2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s" s="13">
+      <c r="E2" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="G2" t="s" s="11">
+      <c r="G2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H2" t="s" s="13">
+      <c r="H2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I2" t="s" s="13">
+      <c r="I2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J2" t="s" s="13">
+      <c r="J2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K2" t="s" s="13">
+      <c r="K2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L2" t="s" s="13">
+      <c r="L2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M2" t="s" s="13">
+      <c r="M2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N2" t="s" s="13">
+      <c r="N2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="O2" t="s" s="13">
+      <c r="O2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="P2" t="s" s="13">
+      <c r="P2" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="13">
+    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" t="s" s="13">
+      <c r="D3" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="8"/>
-      <c r="G3" t="s" s="11">
+      <c r="G3" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="4"/>
@@ -2395,14 +2443,14 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="8"/>
-      <c r="G4" t="s" s="11">
+      <c r="G4" s="10" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="4"/>
@@ -2411,18 +2459,18 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="15"/>
+      <c r="N4" s="13"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="8"/>
-      <c r="G5" t="s" s="11">
+      <c r="G5" s="10" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="4"/>
@@ -2435,7 +2483,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2453,7 +2501,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2471,7 +2519,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2489,7 +2537,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2507,7 +2555,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2527,7 +2575,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Validate digestion method when updating proteomics measurements (#565)
* fix typos in digestion method preselection

* validate digestion methods when updating measurements

* use equals ignore
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,19 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124864F-3DCA-2740-A285-737260ED93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="26080" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Metadata" sheetId="1" r:id="rId4"/>
-    <sheet name="Property information" sheetId="2" r:id="rId5"/>
-    <sheet name="Allowed values" sheetId="3" r:id="rId6"/>
+    <sheet name="Metadata" sheetId="1" r:id="rId1"/>
+    <sheet name="Property information" sheetId="2" r:id="rId2"/>
+    <sheet name="Allowed values" sheetId="3" r:id="rId3"/>
   </sheets>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -171,34 +180,22 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="0" formatCode="General"/>
-  </numFmts>
-  <fonts count="7">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color indexed="8"/>
-      <name val="Helvetica Neue"/>
-    </font>
-    <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="12"/>
       <color indexed="8"/>
       <name val="Aptos Narrow"/>
@@ -207,12 +204,14 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -284,59 +283,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
+  </cellStyleXfs>
+  <cellXfs count="14">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-  </cellStyleXfs>
-  <cellXfs count="16">
-    <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -345,25 +310,85 @@
   <tableStyles count="0"/>
   <colors>
     <indexedColors>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffff0000"/>
-      <rgbColor rgb="ff00ff00"/>
-      <rgbColor rgb="ff0000ff"/>
-      <rgbColor rgb="ffffff00"/>
-      <rgbColor rgb="ffff00ff"/>
-      <rgbColor rgb="ff00ffff"/>
-      <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffaaaaaa"/>
-      <rgbColor rgb="ffa7a7a7"/>
-      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FF00FF00"/>
+      <rgbColor rgb="FF0000FF"/>
+      <rgbColor rgb="FFFFFF00"/>
+      <rgbColor rgb="FFFF00FF"/>
+      <rgbColor rgb="FF00FFFF"/>
+      <rgbColor rgb="FF000000"/>
+      <rgbColor rgb="FFAAAAAA"/>
+      <rgbColor rgb="FFA7A7A7"/>
+      <rgbColor rgb="FFFFFFFF"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office Theme">
       <a:dk1>
@@ -565,7 +590,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -583,7 +608,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -612,7 +637,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -637,7 +662,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -662,7 +687,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -687,7 +712,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -712,7 +737,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -737,7 +762,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -762,7 +787,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -787,7 +812,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -812,7 +837,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -825,9 +850,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:spDef>
@@ -844,7 +875,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:noAutofit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -862,7 +893,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -887,7 +918,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -912,7 +943,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -937,7 +968,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -962,7 +993,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -987,7 +1018,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1012,7 +1043,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1037,7 +1068,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1062,7 +1093,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1087,7 +1118,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1100,9 +1131,15 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:lnDef>
@@ -1116,7 +1153,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1134,7 +1171,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1100" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1163,7 +1200,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1188,7 +1225,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1213,7 +1250,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1238,7 +1275,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1263,7 +1300,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1288,7 +1325,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1313,7 +1350,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1338,7 +1375,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1363,7 +1400,7 @@
           <a:buSzTx/>
           <a:buFontTx/>
           <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1800" u="none" kumimoji="0" normalizeH="0">
+          <a:defRPr kumimoji="0" sz="1800" b="0" i="0" u="none" strike="noStrike" cap="none" spc="0" normalizeH="0" baseline="0">
             <a:ln>
               <a:noFill/>
             </a:ln>
@@ -1376,92 +1413,101 @@
         </a:lvl9pPr>
       </a:lstStyle>
       <a:style>
-        <a:lnRef idx="0"/>
-        <a:fillRef idx="0"/>
-        <a:effectRef idx="0"/>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
         <a:fontRef idx="none"/>
       </a:style>
     </a:txDef>
   </a:objectDefaults>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K2:K33"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="14.8516" style="1" customWidth="1"/>
+    <col min="1" max="2" width="14.83203125" style="1" customWidth="1"/>
     <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6719" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.8516" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6719" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6719" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.3047" style="1" customWidth="1"/>
+    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
+    <col min="5" max="6" width="10.83203125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
     <col min="10" max="10" width="20" style="1" customWidth="1"/>
     <col min="11" max="11" width="16" style="1" customWidth="1"/>
     <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6719" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.8516" style="1" customWidth="1"/>
+    <col min="13" max="13" width="16.6640625" style="1" customWidth="1"/>
+    <col min="14" max="14" width="18.83203125" style="1" customWidth="1"/>
     <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="16" width="10.8516" style="1" customWidth="1"/>
-    <col min="17" max="16384" width="10.8516" style="1" customWidth="1"/>
+    <col min="16" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="17" customHeight="1">
+    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1479,7 +1525,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" ht="17" customHeight="1">
+    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1497,7 +1543,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1515,7 +1561,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1533,7 +1579,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1551,7 +1597,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1569,7 +1615,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1587,7 +1633,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1605,7 +1651,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1623,7 +1669,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" ht="17" customHeight="1">
+    <row r="11" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1641,7 +1687,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" ht="17" customHeight="1">
+    <row r="12" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1659,7 +1705,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" ht="17" customHeight="1">
+    <row r="13" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1677,7 +1723,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" ht="17" customHeight="1">
+    <row r="14" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1695,7 +1741,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" ht="17" customHeight="1">
+    <row r="15" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1713,7 +1759,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" ht="17" customHeight="1">
+    <row r="16" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1731,7 +1777,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" ht="17" customHeight="1">
+    <row r="17" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1749,7 +1795,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" ht="17" customHeight="1">
+    <row r="18" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1767,7 +1813,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" ht="17" customHeight="1">
+    <row r="19" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1785,7 +1831,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" ht="17" customHeight="1">
+    <row r="20" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1803,7 +1849,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" ht="17" customHeight="1">
+    <row r="21" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1821,7 +1867,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" ht="17" customHeight="1">
+    <row r="22" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1839,7 +1885,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" ht="17" customHeight="1">
+    <row r="23" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1857,7 +1903,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" ht="17" customHeight="1">
+    <row r="24" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1875,7 +1921,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" ht="17" customHeight="1">
+    <row r="25" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1893,7 +1939,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" ht="17" customHeight="1">
+    <row r="26" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1911,7 +1957,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" ht="17" customHeight="1">
+    <row r="27" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1929,7 +1975,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" ht="17" customHeight="1">
+    <row r="28" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1947,7 +1993,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" ht="17" customHeight="1">
+    <row r="29" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1965,7 +2011,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" ht="17" customHeight="1">
+    <row r="30" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -1983,7 +2029,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" ht="17" customHeight="1">
+    <row r="31" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2001,7 +2047,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" ht="17" customHeight="1">
+    <row r="32" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2019,7 +2065,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" ht="17" customHeight="1">
+    <row r="33" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2039,12 +2085,12 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K33">
-      <formula1>"in gel,in solition,iST poteomics kit,on beads"</formula1>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K33" xr:uid="{00000000-0002-0000-0000-000000000000}">
+      <formula1>"in gel,in solution,iST proteomics kit,on beads"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2052,200 +2098,201 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="21.1719" style="9" customWidth="1"/>
-    <col min="3" max="3" width="86.1719" style="9" customWidth="1"/>
-    <col min="4" max="16384" width="10.8516" style="9" customWidth="1"/>
+    <col min="1" max="2" width="21.1640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="86.1640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.6" customHeight="1">
-      <c r="A1" t="s" s="10">
+    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B1" t="s" s="10">
+      <c r="B1" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="C1" t="s" s="10">
+      <c r="C1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" ht="13.55" customHeight="1">
-      <c r="A2" t="s" s="11">
+    <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="B2" t="s" s="11">
+      <c r="B2" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C2" t="s" s="11">
+      <c r="C2" s="10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" ht="13.55" customHeight="1">
-      <c r="A3" t="s" s="11">
+    <row r="3" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s" s="11">
+      <c r="B3" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C3" t="s" s="11">
+      <c r="C3" s="10" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" ht="13.55" customHeight="1">
-      <c r="A4" t="s" s="11">
+    <row r="4" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="B4" t="s" s="11">
+      <c r="B4" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s" s="11">
+      <c r="C4" s="10" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="5" ht="13.55" customHeight="1">
-      <c r="A5" t="s" s="11">
+    <row r="5" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="B5" t="s" s="11">
+      <c r="B5" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C5" t="s" s="11">
+      <c r="C5" s="10" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" ht="13.55" customHeight="1">
-      <c r="A6" t="s" s="11">
+    <row r="6" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="B6" t="s" s="11">
+      <c r="B6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C6" t="s" s="11">
+      <c r="C6" s="10" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" ht="17" customHeight="1">
-      <c r="A7" t="s" s="11">
+    <row r="7" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="B7" t="s" s="11">
+      <c r="B7" s="10" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="4"/>
     </row>
-    <row r="8" ht="13.55" customHeight="1">
-      <c r="A8" t="s" s="11">
+    <row r="8" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B8" t="s" s="11">
+      <c r="B8" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C8" t="s" s="11">
+      <c r="C8" s="10" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="9" ht="17" customHeight="1">
-      <c r="A9" t="s" s="11">
+    <row r="9" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="B9" t="s" s="11">
+      <c r="B9" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
-      <c r="A10" t="s" s="11">
+    <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="B10" t="s" s="11">
+      <c r="B10" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C10" s="4"/>
     </row>
-    <row r="11" ht="13.55" customHeight="1">
-      <c r="A11" t="s" s="11">
+    <row r="11" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B11" t="s" s="11">
+      <c r="B11" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C11" t="s" s="11">
+      <c r="C11" s="10" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="12" ht="13.55" customHeight="1">
-      <c r="A12" t="s" s="11">
+    <row r="12" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="B12" t="s" s="11">
+      <c r="B12" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C12" t="s" s="11">
+      <c r="C12" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="13" ht="13.55" customHeight="1">
-      <c r="A13" t="s" s="11">
+    <row r="13" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="B13" t="s" s="11">
+      <c r="B13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C13" t="s" s="11">
+      <c r="C13" s="10" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="14" ht="13.55" customHeight="1">
-      <c r="A14" t="s" s="11">
+    <row r="14" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B14" t="s" s="11">
+      <c r="B14" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="C14" t="s" s="11">
+      <c r="C14" s="10" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="15" ht="13.55" customHeight="1">
-      <c r="A15" t="s" s="11">
+    <row r="15" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s" s="11">
+      <c r="B15" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C15" t="s" s="11">
+      <c r="C15" s="10" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="16" ht="13.55" customHeight="1">
-      <c r="A16" t="s" s="11">
+    <row r="16" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s" s="11">
+      <c r="B16" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C16" t="s" s="11">
+      <c r="C16" s="10" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" ht="17" customHeight="1">
-      <c r="A17" t="s" s="11">
+    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="B17" t="s" s="11">
+      <c r="B17" s="10" t="s">
         <v>22</v>
       </c>
       <c r="C17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>
@@ -2253,136 +2300,137 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:P10"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8333" defaultRowHeight="16" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.3516" style="12" customWidth="1"/>
-    <col min="2" max="4" width="16" style="12" customWidth="1"/>
-    <col min="5" max="5" width="18.6719" style="12" customWidth="1"/>
-    <col min="6" max="7" width="34.5" style="12" customWidth="1"/>
-    <col min="8" max="9" width="17.3516" style="12" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="12" customWidth="1"/>
-    <col min="11" max="11" width="26.1719" style="12" customWidth="1"/>
-    <col min="12" max="12" width="22.8516" style="12" customWidth="1"/>
-    <col min="13" max="13" width="17" style="12" customWidth="1"/>
-    <col min="14" max="14" width="24" style="12" customWidth="1"/>
-    <col min="15" max="15" width="10.8516" style="12" customWidth="1"/>
-    <col min="16" max="16" width="12.1719" style="12" customWidth="1"/>
-    <col min="17" max="16384" width="10.8516" style="12" customWidth="1"/>
+    <col min="1" max="1" width="30.33203125" style="1" customWidth="1"/>
+    <col min="2" max="4" width="16" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
+    <col min="6" max="7" width="34.5" style="1" customWidth="1"/>
+    <col min="8" max="9" width="17.33203125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
+    <col min="11" max="11" width="26.1640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="22.83203125" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17" style="1" customWidth="1"/>
+    <col min="14" max="14" width="24" style="1" customWidth="1"/>
+    <col min="15" max="15" width="10.83203125" style="1" customWidth="1"/>
+    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="1" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="13.55" customHeight="1">
-      <c r="A1" t="s" s="2">
+    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s" s="2">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s" s="2">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s" s="3">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s" s="2">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s" s="2">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s" s="2">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s" s="2">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s" s="2">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s" s="2">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s" s="2">
+      <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s" s="2">
+      <c r="L1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s" s="2">
+      <c r="M1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s" s="2">
+      <c r="N1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s" s="2">
+      <c r="O1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s" s="2">
+      <c r="P1" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" ht="17" customHeight="1">
-      <c r="A2" t="s" s="13">
+    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="B2" t="s" s="13">
+      <c r="B2" s="11" t="s">
         <v>42</v>
       </c>
       <c r="C2" s="4"/>
-      <c r="D2" t="s" s="14">
+      <c r="D2" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="E2" t="s" s="13">
+      <c r="E2" s="11" t="s">
         <v>42</v>
       </c>
       <c r="F2" s="8"/>
-      <c r="G2" t="s" s="11">
+      <c r="G2" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="H2" t="s" s="13">
+      <c r="H2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="I2" t="s" s="13">
+      <c r="I2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="J2" t="s" s="13">
+      <c r="J2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="K2" t="s" s="13">
+      <c r="K2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="L2" t="s" s="13">
+      <c r="L2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="M2" t="s" s="13">
+      <c r="M2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="N2" t="s" s="13">
+      <c r="N2" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="O2" t="s" s="13">
+      <c r="O2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="P2" t="s" s="13">
+      <c r="P2" s="11" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" ht="17" customHeight="1">
-      <c r="A3" t="s" s="13">
+    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="11" t="s">
         <v>46</v>
       </c>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
-      <c r="D3" t="s" s="13">
+      <c r="D3" s="11" t="s">
         <v>47</v>
       </c>
       <c r="E3" s="4"/>
       <c r="F3" s="8"/>
-      <c r="G3" t="s" s="11">
+      <c r="G3" s="10" t="s">
         <v>48</v>
       </c>
       <c r="H3" s="4"/>
@@ -2395,14 +2443,14 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" ht="17" customHeight="1">
+    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
       <c r="E4" s="4"/>
       <c r="F4" s="8"/>
-      <c r="G4" t="s" s="11">
+      <c r="G4" s="10" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="4"/>
@@ -2411,18 +2459,18 @@
       <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
-      <c r="N4" s="15"/>
+      <c r="N4" s="13"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" ht="17" customHeight="1">
+    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
       <c r="F5" s="8"/>
-      <c r="G5" t="s" s="11">
+      <c r="G5" s="10" t="s">
         <v>50</v>
       </c>
       <c r="H5" s="4"/>
@@ -2435,7 +2483,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" ht="17" customHeight="1">
+    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -2453,7 +2501,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" ht="17" customHeight="1">
+    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -2471,7 +2519,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" ht="17" customHeight="1">
+    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -2489,7 +2537,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" ht="17" customHeight="1">
+    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -2507,7 +2555,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" ht="17" customHeight="1">
+    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -2527,7 +2575,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="100" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
+  <pageSetup orientation="portrait"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>

<commit_message>
Update NGS and PXP template
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124864F-3DCA-2740-A285-737260ED93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40B5677-173D-F748-B2B0-4D73BC587DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26080" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Property information" sheetId="2" r:id="rId2"/>
-    <sheet name="Allowed values" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -63,12 +62,6 @@
     <t>Enrichment Method</t>
   </si>
   <si>
-    <t>Injection Volume (uL)*</t>
-  </si>
-  <si>
-    <t>LCMS Method*</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -81,9 +74,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>QBiC Sample Id</t>
-  </si>
-  <si>
     <t>mandatory</t>
   </si>
   <si>
@@ -93,36 +83,12 @@
     <t>optional</t>
   </si>
   <si>
-    <t>This is just a visual aid simplify sample navigation. This column gets ignored during measurement registration</t>
-  </si>
-  <si>
-    <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
-  </si>
-  <si>
-    <t>Organisation</t>
-  </si>
-  <si>
     <t>For good provenance tracking and enabling FAIR, we need a persistent and unique identifier of the organisation the measurement has been conducted at. We expect a full ROR id as URL (e.g. https://ror.org/03a1kwz48)</t>
   </si>
   <si>
-    <t>Facility</t>
-  </si>
-  <si>
     <t>Ideally the facilites name within the organisation (groupname, etc.)</t>
   </si>
   <si>
-    <t>LC Column</t>
-  </si>
-  <si>
-    <t>Instrument</t>
-  </si>
-  <si>
-    <t>The instrument model that has been used for the measurement</t>
-  </si>
-  <si>
-    <t>Some times a sample is fractionated and all 7 fractions are measured.</t>
-  </si>
-  <si>
     <t>Digestion Method</t>
   </si>
   <si>
@@ -147,41 +113,50 @@
     <t>LCMS Method</t>
   </si>
   <si>
-    <t>QBiC sample id</t>
-  </si>
-  <si>
     <t>free text</t>
   </si>
   <si>
-    <t>full ROR url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">number </t>
-  </si>
-  <si>
-    <t>(e.g. QTEST001AE)</t>
-  </si>
-  <si>
-    <t>https://ror.org/</t>
-  </si>
-  <si>
-    <t>Currently supported ontologies:</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ols4/ontologies/efo</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ols4/ontologies/ms</t>
+    <t>This is just a visual aid simplify sample navigation for the person managing the metadata. You can e.g. download the sample metadata and copy the sample ID + label column in here. This column gets ignored during measurement registration</t>
+  </si>
+  <si>
+    <t>In case of multiple sample are pooled for measurement, indicate with a common sample pool group label for samples that are in the same measurement. Entries that share the same pool label are recognised as a pool and assigned only one measurement ID and the sample id references remain conserved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The label type that has been used to label the sample for measurement </t>
+  </si>
+  <si>
+    <t>Organisation*</t>
+  </si>
+  <si>
+    <t>The instrument model that has been used for the measurement, which needs to be an ontology CURIE that will be resolved to an existing persistent ID. You can use the ontology search in the data manager to get the CURIE for an instrument model.</t>
+  </si>
+  <si>
+    <t>The label value for the label type that has been used</t>
+  </si>
+  <si>
+    <t>Sometimes a sample is fractionated and all fractions are measured. With this property you can indicate wich fraction it is.</t>
+  </si>
+  <si>
+    <t>Allowed values</t>
+  </si>
+  <si>
+    <t>QBiC sample ids</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>CURIE</t>
+  </si>
+  <si>
+    <t>whole number</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -189,29 +164,19 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Open Sans Regular"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Open Sans Regular"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <name val="Open Sans Regular"/>
     </font>
   </fonts>
   <fills count="3">
@@ -285,23 +250,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,30 +1396,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K2:K33"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="2" width="14.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="17" width="10.83203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="5" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1467,7 +1432,7 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="10" t="s">
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -1498,20 +1463,20 @@
         <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
+      <c r="D2" s="7"/>
       <c r="E2" s="4"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
@@ -1519,13 +1484,13 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4"/>
-      <c r="L2" s="6"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1543,7 +1508,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1561,7 +1526,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1579,7 +1544,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1597,7 +1562,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1615,7 +1580,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1633,7 +1598,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1651,7 +1616,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1669,7 +1634,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1687,7 +1652,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1705,7 +1670,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1723,7 +1688,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1741,7 +1706,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1759,7 +1724,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1771,13 +1736,13 @@
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
       <c r="K16" s="4"/>
-      <c r="L16" s="7"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1789,13 +1754,13 @@
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
       <c r="K17" s="4"/>
-      <c r="L17" s="8"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1807,13 +1772,13 @@
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
       <c r="K18" s="4"/>
-      <c r="L18" s="8"/>
+      <c r="L18" s="6"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1825,13 +1790,13 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="4"/>
-      <c r="L19" s="8"/>
+      <c r="L19" s="6"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1843,13 +1808,13 @@
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
       <c r="K20" s="4"/>
-      <c r="L20" s="8"/>
+      <c r="L20" s="6"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1861,13 +1826,13 @@
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
       <c r="K21" s="4"/>
-      <c r="L21" s="8"/>
+      <c r="L21" s="6"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1879,13 +1844,13 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="4"/>
-      <c r="L22" s="8"/>
+      <c r="L22" s="6"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1897,13 +1862,13 @@
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
       <c r="K23" s="4"/>
-      <c r="L23" s="8"/>
+      <c r="L23" s="6"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1915,13 +1880,13 @@
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
       <c r="K24" s="4"/>
-      <c r="L24" s="8"/>
+      <c r="L24" s="6"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1933,13 +1898,13 @@
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
       <c r="K25" s="4"/>
-      <c r="L25" s="8"/>
+      <c r="L25" s="6"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1951,13 +1916,13 @@
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
       <c r="K26" s="4"/>
-      <c r="L26" s="8"/>
+      <c r="L26" s="6"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1969,13 +1934,13 @@
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
       <c r="K27" s="4"/>
-      <c r="L27" s="8"/>
+      <c r="L27" s="6"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1987,13 +1952,13 @@
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
-      <c r="L28" s="8"/>
+      <c r="L28" s="6"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2005,13 +1970,13 @@
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
-      <c r="L29" s="8"/>
+      <c r="L29" s="6"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2023,13 +1988,13 @@
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
       <c r="K30" s="4"/>
-      <c r="L30" s="8"/>
+      <c r="L30" s="6"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2041,13 +2006,13 @@
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
       <c r="K31" s="4"/>
-      <c r="L31" s="8"/>
+      <c r="L31" s="6"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2059,13 +2024,13 @@
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
       <c r="K32" s="4"/>
-      <c r="L32" s="8"/>
+      <c r="L32" s="6"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2077,7 +2042,7 @@
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
       <c r="K33" s="4"/>
-      <c r="L33" s="8"/>
+      <c r="L33" s="6"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -2099,479 +2064,255 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="21.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="86.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="37" style="1" customWidth="1"/>
+    <col min="4" max="4" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="19">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="19">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="3" spans="1:4" ht="19">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19">
+      <c r="A5" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="6" spans="1:4" ht="19">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="7" spans="1:4" ht="19">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D7" s="4"/>
+    </row>
+    <row r="8" spans="1:4" ht="19">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19">
+      <c r="A9" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19">
+      <c r="A10" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D10" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19">
+      <c r="A11" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19">
+      <c r="A12" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="10" t="s">
+    <row r="13" spans="1:4" ht="19">
+      <c r="A13" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
+      <c r="B13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="10" t="s">
+    </row>
+    <row r="14" spans="1:4" ht="19">
+      <c r="A14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
+    <row r="15" spans="1:4" ht="19">
+      <c r="A15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="10" t="s">
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
+    <row r="16" spans="1:4" ht="19">
+      <c r="A16" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.33203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="34.5" style="1" customWidth="1"/>
-    <col min="8" max="9" width="17.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="D16" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19">
+      <c r="A17" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D17" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Injection volume and LCMS method not mandatory anymore
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F40B5677-173D-F748-B2B0-4D73BC587DA2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E486C2FE-7037-F243-87F0-BE0126C9AC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="1680" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -150,6 +150,12 @@
   </si>
   <si>
     <t>whole number</t>
+  </si>
+  <si>
+    <t>enumeration</t>
+  </si>
+  <si>
+    <t>The digestion method used, one of: 'in gel', 'in solution', 'iST proteomics kit', 'on beads'</t>
   </si>
 </sst>
 </file>
@@ -2067,7 +2073,7 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
@@ -2240,10 +2246,10 @@
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19">

</xml_diff>

<commit_message>
Update proteomics measurement template
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E486C2FE-7037-F243-87F0-BE0126C9AC1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3208C87-9E67-844E-A5D8-AD1544DE6519}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38400" yWindow="1680" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -89,27 +89,9 @@
     <t>Ideally the facilites name within the organisation (groupname, etc.)</t>
   </si>
   <si>
-    <t>Digestion Method</t>
-  </si>
-  <si>
-    <t>Recovery of proteins differed between methods</t>
-  </si>
-  <si>
-    <t>Digestion Enzyme</t>
-  </si>
-  <si>
-    <t>Information on how many cycles for each read and index</t>
-  </si>
-  <si>
-    <t>the method leading to multiple  cycles or fractions (see Cycle/Fraction Name)</t>
-  </si>
-  <si>
     <t>Injection Volume (uL)</t>
   </si>
   <si>
-    <t>Commenting notes about the measurement</t>
-  </si>
-  <si>
     <t>LCMS Method</t>
   </si>
   <si>
@@ -146,23 +128,41 @@
     <t>URL</t>
   </si>
   <si>
-    <t>CURIE</t>
-  </si>
-  <si>
     <t>whole number</t>
   </si>
   <si>
     <t>enumeration</t>
   </si>
   <si>
-    <t>The digestion method used, one of: 'in gel', 'in solution', 'iST proteomics kit', 'on beads'</t>
+    <t>CURIE (ontology)</t>
+  </si>
+  <si>
+    <t>Method that has been used to break proteins into peptides. One of: 'in gel', 'in solution', 'iST proteomics kit', 'on beads'</t>
+  </si>
+  <si>
+    <t>Information about the used enzymes for the proteolitic .</t>
+  </si>
+  <si>
+    <t>The type of column that has been used.  You can use the commercial name or brand .</t>
+  </si>
+  <si>
+    <t>Enrichment of proteins or peptides of different charecteristics.</t>
+  </si>
+  <si>
+    <t>Laboratory specific methods that have been used for LCMS measurements.</t>
+  </si>
+  <si>
+    <t>Notes about the measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sample volume injected into the LC column in microliter  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -182,6 +182,10 @@
     <font>
       <sz val="11"/>
       <color indexed="8"/>
+      <name val="Open Sans Regular"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <name val="Open Sans Regular"/>
     </font>
   </fonts>
@@ -256,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
@@ -270,6 +274,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1402,8 +1407,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+    <sheetView showGridLines="0" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
@@ -1411,18 +1416,18 @@
     <col min="1" max="1" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="10.83203125" style="5" customWidth="1"/>
     <col min="18" max="16384" width="10.83203125" style="5"/>
@@ -1438,41 +1443,41 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>27</v>
-      </c>
       <c r="O1" s="2" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="P1" s="2" t="s">
         <v>13</v>
@@ -1482,15 +1487,15 @@
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
@@ -1741,8 +1746,8 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="9"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1759,8 +1764,8 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="6"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1777,8 +1782,8 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="6"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1795,8 +1800,8 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="6"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1813,8 +1818,8 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="6"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1831,8 +1836,8 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="6"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1849,8 +1854,8 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="6"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -1867,8 +1872,8 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="6"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -1885,8 +1890,8 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="6"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
@@ -1903,8 +1908,8 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="6"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
@@ -1921,8 +1926,8 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="6"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
@@ -1939,8 +1944,8 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="6"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
@@ -1957,8 +1962,8 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="6"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
@@ -1975,8 +1980,8 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="6"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -1993,8 +1998,8 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="6"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -2011,8 +2016,8 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="6"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -2029,8 +2034,8 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="6"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
@@ -2047,8 +2052,8 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="6"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -2056,7 +2061,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K33" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J33" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"in gel,in solution,iST proteomics kit,on beads"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2073,15 +2078,15 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="37" style="1" customWidth="1"/>
-    <col min="4" max="4" width="255.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="162.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
@@ -2094,7 +2099,7 @@
         <v>15</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>16</v>
@@ -2108,7 +2113,7 @@
         <v>17</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>18</v>
@@ -2122,10 +2127,10 @@
         <v>19</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="19">
@@ -2136,176 +2141,178 @@
         <v>19</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="19">
       <c r="A5" s="3" t="s">
-        <v>34</v>
+        <v>9</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="19">
       <c r="A6" s="3" t="s">
-        <v>4</v>
+        <v>28</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19">
       <c r="A7" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D7" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="8" spans="1:4" ht="19">
       <c r="A8" s="3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>35</v>
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19">
       <c r="A9" s="3" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>37</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="19">
       <c r="A10" s="3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10" s="4" t="s">
-        <v>33</v>
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="19">
       <c r="A11" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>30</v>
+        <v>36</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="19">
       <c r="A12" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>44</v>
+        <v>24</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="19">
       <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>30</v>
-      </c>
       <c r="D13" s="3" t="s">
-        <v>25</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="19">
       <c r="A14" s="3" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D14" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="19">
       <c r="A15" s="3" t="s">
-        <v>27</v>
+        <v>8</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>28</v>
+        <v>24</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="19">
       <c r="A16" s="3" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>23</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="19">
@@ -2316,9 +2323,11 @@
         <v>19</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D17" s="4"/>
+        <v>24</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>43</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Update metadata requirements for measurements (#577)
* Update NGS and PXP template

* Injection volume and LCMS method not mandatory anymore

* Allow empty values for injection volume

* Remove tests for now optional fields

* Update proteomics measurement template

* Correct grammar

---------

Co-authored-by: Tobias Koch <tobias.koch@qbic.uni-tuebingen.de>
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10512"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sven1103/git/data-manager/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4124864F-3DCA-2740-A285-737260ED93DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48B887B4-D75D-4C41-83C5-C7E9BB702247}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="26080" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38400" yWindow="1680" windowWidth="28800" windowHeight="17500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
     <sheet name="Property information" sheetId="2" r:id="rId2"/>
-    <sheet name="Allowed values" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -63,12 +62,6 @@
     <t>Enrichment Method</t>
   </si>
   <si>
-    <t>Injection Volume (uL)*</t>
-  </si>
-  <si>
-    <t>LCMS Method*</t>
-  </si>
-  <si>
     <t>Comment</t>
   </si>
   <si>
@@ -81,9 +74,6 @@
     <t>Description</t>
   </si>
   <si>
-    <t>QBiC Sample Id</t>
-  </si>
-  <si>
     <t>mandatory</t>
   </si>
   <si>
@@ -93,95 +83,83 @@
     <t>optional</t>
   </si>
   <si>
-    <t>This is just a visual aid simplify sample navigation. This column gets ignored during measurement registration</t>
-  </si>
-  <si>
-    <t>In case of pooled sample get measuremed, indicate with a common sample group label for samples that are in the same measurement. Entries that share the same pool label will be combined as one measurement</t>
-  </si>
-  <si>
-    <t>Organisation</t>
-  </si>
-  <si>
     <t>For good provenance tracking and enabling FAIR, we need a persistent and unique identifier of the organisation the measurement has been conducted at. We expect a full ROR id as URL (e.g. https://ror.org/03a1kwz48)</t>
   </si>
   <si>
-    <t>Facility</t>
-  </si>
-  <si>
     <t>Ideally the facilites name within the organisation (groupname, etc.)</t>
   </si>
   <si>
-    <t>LC Column</t>
-  </si>
-  <si>
-    <t>Instrument</t>
-  </si>
-  <si>
-    <t>The instrument model that has been used for the measurement</t>
-  </si>
-  <si>
-    <t>Some times a sample is fractionated and all 7 fractions are measured.</t>
-  </si>
-  <si>
-    <t>Digestion Method</t>
-  </si>
-  <si>
-    <t>Recovery of proteins differed between methods</t>
-  </si>
-  <si>
-    <t>Digestion Enzyme</t>
-  </si>
-  <si>
-    <t>Information on how many cycles for each read and index</t>
-  </si>
-  <si>
-    <t>the method leading to multiple  cycles or fractions (see Cycle/Fraction Name)</t>
-  </si>
-  <si>
     <t>Injection Volume (uL)</t>
   </si>
   <si>
-    <t>Commenting notes about the measurement</t>
-  </si>
-  <si>
     <t>LCMS Method</t>
   </si>
   <si>
-    <t>QBiC sample id</t>
-  </si>
-  <si>
     <t>free text</t>
   </si>
   <si>
-    <t>full ROR url</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ontology CURIE (e.g. EFO:0008637) </t>
-  </si>
-  <si>
-    <t xml:space="preserve">number </t>
-  </si>
-  <si>
-    <t>(e.g. QTEST001AE)</t>
-  </si>
-  <si>
-    <t>https://ror.org/</t>
-  </si>
-  <si>
-    <t>Currently supported ontologies:</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ols4/ontologies/efo</t>
-  </si>
-  <si>
-    <t>https://www.ebi.ac.uk/ols4/ontologies/ms</t>
+    <t>This is just a visual aid simplify sample navigation for the person managing the metadata. You can e.g. download the sample metadata and copy the sample ID + label column in here. This column gets ignored during measurement registration</t>
+  </si>
+  <si>
+    <t>In case of multiple sample are pooled for measurement, indicate with a common sample pool group label for samples that are in the same measurement. Entries that share the same pool label are recognised as a pool and assigned only one measurement ID and the sample id references remain conserved</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The label type that has been used to label the sample for measurement </t>
+  </si>
+  <si>
+    <t>The instrument model that has been used for the measurement, which needs to be an ontology CURIE that will be resolved to an existing persistent ID. You can use the ontology search in the data manager to get the CURIE for an instrument model.</t>
+  </si>
+  <si>
+    <t>The label value for the label type that has been used</t>
+  </si>
+  <si>
+    <t>Sometimes a sample is fractionated and all fractions are measured. With this property you can indicate wich fraction it is.</t>
+  </si>
+  <si>
+    <t>Allowed values</t>
+  </si>
+  <si>
+    <t>QBiC sample ids</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>whole number</t>
+  </si>
+  <si>
+    <t>enumeration</t>
+  </si>
+  <si>
+    <t>CURIE (ontology)</t>
+  </si>
+  <si>
+    <t>Method that has been used to break proteins into peptides. One of: 'in gel', 'in solution', 'iST proteomics kit', 'on beads'</t>
+  </si>
+  <si>
+    <t>Information about the used enzymes for the proteolitic .</t>
+  </si>
+  <si>
+    <t>The type of column that has been used.  You can use the commercial name or brand .</t>
+  </si>
+  <si>
+    <t>Enrichment of proteins or peptides of different charecteristics.</t>
+  </si>
+  <si>
+    <t>Laboratory specific methods that have been used for LCMS measurements.</t>
+  </si>
+  <si>
+    <t>Notes about the measurement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The sample volume injected into the LC column in microliter  </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -189,29 +167,23 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="12"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Open Sans Regular"/>
     </font>
     <font>
-      <b/>
       <sz val="12"/>
       <color indexed="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Open Sans Regular"/>
     </font>
     <font>
       <sz val="11"/>
       <color indexed="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="Open Sans Regular"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
+      <sz val="12"/>
+      <name val="Open Sans Regular"/>
     </font>
   </fonts>
   <fills count="3">
@@ -285,23 +257,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1434,30 +1404,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P33"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K4" sqref="K2:K33"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="R5" sqref="R5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
-    <col min="1" max="2" width="14.83203125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="1" customWidth="1"/>
-    <col min="4" max="4" width="14.6640625" style="1" customWidth="1"/>
-    <col min="5" max="6" width="10.83203125" style="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" style="1" customWidth="1"/>
-    <col min="8" max="8" width="11.6640625" style="1" customWidth="1"/>
-    <col min="9" max="9" width="12.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="20" style="1" customWidth="1"/>
-    <col min="11" max="11" width="16" style="1" customWidth="1"/>
-    <col min="12" max="12" width="19" style="1" customWidth="1"/>
-    <col min="13" max="13" width="16.6640625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="18.83203125" style="1" customWidth="1"/>
-    <col min="15" max="15" width="13" style="1" customWidth="1"/>
-    <col min="16" max="17" width="10.83203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.83203125" style="5" customWidth="1"/>
+    <col min="18" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1467,65 +1440,65 @@
       <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="10" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="P1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:16">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="4"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="6"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1543,7 +1516,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1561,7 +1534,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1579,7 +1552,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1597,7 +1570,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1615,7 +1588,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1633,7 +1606,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1651,7 +1624,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1669,7 +1642,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1687,7 +1660,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1705,7 +1678,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1723,7 +1696,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1741,7 +1714,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1759,7 +1732,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1770,14 +1743,14 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="4"/>
-      <c r="L16" s="7"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="4"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1788,14 +1761,14 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="4"/>
-      <c r="L17" s="8"/>
+      <c r="K17" s="6"/>
+      <c r="L17" s="4"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1806,14 +1779,14 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="4"/>
-      <c r="L18" s="8"/>
+      <c r="K18" s="6"/>
+      <c r="L18" s="4"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1824,14 +1797,14 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="4"/>
-      <c r="L19" s="8"/>
+      <c r="K19" s="6"/>
+      <c r="L19" s="4"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1842,14 +1815,14 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="8"/>
+      <c r="K20" s="6"/>
+      <c r="L20" s="4"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1860,14 +1833,14 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="4"/>
-      <c r="L21" s="8"/>
+      <c r="K21" s="6"/>
+      <c r="L21" s="4"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1878,14 +1851,14 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
-      <c r="L22" s="8"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="4"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1896,14 +1869,14 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="4"/>
-      <c r="L23" s="8"/>
+      <c r="K23" s="6"/>
+      <c r="L23" s="4"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1914,14 +1887,14 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="4"/>
-      <c r="L24" s="8"/>
+      <c r="K24" s="6"/>
+      <c r="L24" s="4"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1932,14 +1905,14 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="4"/>
-      <c r="L25" s="8"/>
+      <c r="K25" s="6"/>
+      <c r="L25" s="4"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1950,14 +1923,14 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="4"/>
-      <c r="L26" s="8"/>
+      <c r="K26" s="6"/>
+      <c r="L26" s="4"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1968,14 +1941,14 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="4"/>
-      <c r="L27" s="8"/>
+      <c r="K27" s="6"/>
+      <c r="L27" s="4"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1986,14 +1959,14 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="4"/>
-      <c r="L28" s="8"/>
+      <c r="K28" s="6"/>
+      <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -2004,14 +1977,14 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
-      <c r="L29" s="8"/>
+      <c r="K29" s="6"/>
+      <c r="L29" s="4"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2022,14 +1995,14 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="4"/>
-      <c r="L30" s="8"/>
+      <c r="K30" s="6"/>
+      <c r="L30" s="4"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2040,14 +2013,14 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="4"/>
-      <c r="L31" s="8"/>
+      <c r="K31" s="6"/>
+      <c r="L31" s="4"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2058,14 +2031,14 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="4"/>
-      <c r="L32" s="8"/>
+      <c r="K32" s="6"/>
+      <c r="L32" s="4"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2076,8 +2049,8 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="4"/>
-      <c r="L33" s="8"/>
+      <c r="K33" s="6"/>
+      <c r="L33" s="4"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
@@ -2085,7 +2058,7 @@
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K33" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J33" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"in gel,in solution,iST proteomics kit,on beads"</formula1>
     </dataValidation>
   </dataValidations>
@@ -2099,479 +2072,259 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="21.1640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="86.1640625" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.83203125" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="24.5" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="28.33203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="162.1640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="10.83203125" style="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="14.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="9" t="s">
+    <row r="1" spans="1:4" ht="19">
+      <c r="A1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="9" t="s">
+    </row>
+    <row r="2" spans="1:4" ht="19">
+      <c r="A2" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+    <row r="3" spans="1:4" ht="19">
+      <c r="A3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="C3" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19">
+      <c r="A5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19">
+      <c r="A6" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="10" t="s">
+    </row>
+    <row r="7" spans="1:4" ht="19">
+      <c r="A7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="10" t="s">
+    <row r="8" spans="1:4" ht="19">
+      <c r="A8" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19">
+      <c r="A9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19">
+      <c r="A10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="19">
+      <c r="A11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19">
+      <c r="A12" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D12" s="11" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="19">
+      <c r="A13" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="19">
+      <c r="A14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="19">
+      <c r="A15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="19">
+      <c r="A16" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" s="10" t="s">
+      <c r="B16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="19">
+      <c r="A17" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C17" s="3" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" s="10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="10" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C7" s="4"/>
-    </row>
-    <row r="8" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="10" t="s">
-        <v>30</v>
-      </c>
-      <c r="B8" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C8" s="10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" s="4"/>
-    </row>
-    <row r="10" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="10" t="s">
-        <v>7</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C10" s="4"/>
-    </row>
-    <row r="11" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="10" t="s">
-        <v>35</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="10" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="B15" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C15" s="10" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="B16" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="10" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="10" t="s">
-        <v>22</v>
-      </c>
-      <c r="C17" s="4"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <headerFooter>
-    <oddFooter>&amp;C&amp;"Helvetica Neue,Regular"&amp;12&amp;K000000&amp;P</oddFooter>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:P10"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="30.33203125" style="1" customWidth="1"/>
-    <col min="2" max="4" width="16" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.6640625" style="1" customWidth="1"/>
-    <col min="6" max="7" width="34.5" style="1" customWidth="1"/>
-    <col min="8" max="9" width="17.33203125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="17.5" style="1" customWidth="1"/>
-    <col min="11" max="11" width="26.1640625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="22.83203125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17" style="1" customWidth="1"/>
-    <col min="14" max="14" width="24" style="1" customWidth="1"/>
-    <col min="15" max="15" width="10.83203125" style="1" customWidth="1"/>
-    <col min="16" max="16" width="12.1640625" style="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="1" customWidth="1"/>
-    <col min="18" max="16384" width="10.83203125" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:16" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="B2" s="11" t="s">
+      <c r="D17" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C2" s="4"/>
-      <c r="D2" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="E2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="F2" s="8"/>
-      <c r="G2" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="L2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="M2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="N2" s="11" t="s">
-        <v>45</v>
-      </c>
-      <c r="O2" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="P2" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="4"/>
-      <c r="C3" s="4"/>
-      <c r="D3" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="E3" s="4"/>
-      <c r="F3" s="8"/>
-      <c r="G3" s="10" t="s">
-        <v>48</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4"/>
-      <c r="J3" s="4"/>
-      <c r="K3" s="4"/>
-      <c r="L3" s="4"/>
-      <c r="M3" s="4"/>
-      <c r="N3" s="4"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="10" t="s">
-        <v>49</v>
-      </c>
-      <c r="H4" s="4"/>
-      <c r="I4" s="4"/>
-      <c r="J4" s="4"/>
-      <c r="K4" s="4"/>
-      <c r="L4" s="4"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="13"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="H5" s="4"/>
-      <c r="I5" s="4"/>
-      <c r="J5" s="4"/>
-      <c r="K5" s="4"/>
-      <c r="L5" s="4"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
-      <c r="I6" s="4"/>
-      <c r="J6" s="4"/>
-      <c r="K6" s="4"/>
-      <c r="L6" s="4"/>
-      <c r="M6" s="4"/>
-      <c r="N6" s="4"/>
-      <c r="O6" s="4"/>
-      <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
-      <c r="I7" s="4"/>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4"/>
-      <c r="L7" s="4"/>
-      <c r="M7" s="4"/>
-      <c r="N7" s="4"/>
-      <c r="O7" s="4"/>
-      <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="4"/>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
-      <c r="L8" s="4"/>
-      <c r="M8" s="4"/>
-      <c r="N8" s="4"/>
-      <c r="O8" s="4"/>
-      <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="4"/>
-      <c r="B9" s="4"/>
-      <c r="C9" s="4"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
-      <c r="H9" s="4"/>
-      <c r="I9" s="4"/>
-      <c r="J9" s="4"/>
-      <c r="K9" s="4"/>
-      <c r="L9" s="4"/>
-      <c r="M9" s="4"/>
-      <c r="N9" s="4"/>
-      <c r="O9" s="4"/>
-      <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16" ht="17" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4"/>
-      <c r="B10" s="4"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
-      <c r="H10" s="4"/>
-      <c r="I10" s="4"/>
-      <c r="J10" s="4"/>
-      <c r="K10" s="4"/>
-      <c r="L10" s="4"/>
-      <c r="M10" s="4"/>
-      <c r="N10" s="4"/>
-      <c r="O10" s="4"/>
-      <c r="P10" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Rename `Instrument` to `MS Device` in template
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10908"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/afriedrich/git/data-manager-app/user-interface/src/main/resources/templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kocht/SoftwareDevelopment/portlets/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F322614E-D130-EC47-9A09-935515B4CE34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C738A0D3-FE3F-8248-A163-3349CA2A65DB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="1680" windowWidth="28800" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="45">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -153,13 +153,16 @@
   </si>
   <si>
     <t>Sample Name</t>
+  </si>
+  <si>
+    <t>MS Device*</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -1405,10 +1408,10 @@
   <dimension ref="A1:P33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="19"/>
   <cols>
     <col min="1" max="1" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
@@ -1430,7 +1433,7 @@
     <col min="18" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1453,7 +1456,7 @@
         <v>4</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>5</v>
+        <v>44</v>
       </c>
       <c r="I1" s="2" t="s">
         <v>22</v>
@@ -1480,7 +1483,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
@@ -1498,7 +1501,7 @@
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1516,7 +1519,7 @@
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1534,7 +1537,7 @@
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1552,7 +1555,7 @@
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:16">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1570,7 +1573,7 @@
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:16">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1588,7 +1591,7 @@
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1606,7 +1609,7 @@
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1624,7 +1627,7 @@
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:16">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1642,7 +1645,7 @@
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1660,7 +1663,7 @@
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1678,7 +1681,7 @@
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:16">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1696,7 +1699,7 @@
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1714,7 +1717,7 @@
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:16">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1732,7 +1735,7 @@
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1750,7 +1753,7 @@
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:16">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1768,7 +1771,7 @@
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
     </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:16">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1786,7 +1789,7 @@
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:16">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1804,7 +1807,7 @@
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:16">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1822,7 +1825,7 @@
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:16">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1840,7 +1843,7 @@
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:16">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1858,7 +1861,7 @@
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
     </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:16">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1876,7 +1879,7 @@
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:16">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1894,7 +1897,7 @@
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:16">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1912,7 +1915,7 @@
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:16">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1930,7 +1933,7 @@
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:16">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1948,7 +1951,7 @@
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:16">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1966,7 +1969,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
     </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:16">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1984,7 +1987,7 @@
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:16">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2002,7 +2005,7 @@
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:16">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2020,7 +2023,7 @@
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:16">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2038,7 +2041,7 @@
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
     </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:16">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2078,7 +2081,7 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.83203125" defaultRowHeight="16" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="24.5" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.33203125" style="1" bestFit="1" customWidth="1"/>
@@ -2088,7 +2091,7 @@
     <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="16" customHeight="1">
       <c r="A1" s="2" t="s">
         <v>13</v>
       </c>
@@ -2102,7 +2105,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" ht="16" customHeight="1">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -2116,7 +2119,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="16" customHeight="1">
       <c r="A3" s="3" t="s">
         <v>43</v>
       </c>
@@ -2130,7 +2133,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="16" customHeight="1">
       <c r="A4" s="3" t="s">
         <v>1</v>
       </c>
@@ -2144,7 +2147,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="16" customHeight="1">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -2158,7 +2161,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" ht="16" customHeight="1">
       <c r="A6" s="3" t="s">
         <v>2</v>
       </c>
@@ -2172,7 +2175,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" ht="16" customHeight="1">
       <c r="A7" s="3" t="s">
         <v>3</v>
       </c>
@@ -2186,7 +2189,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="16" customHeight="1">
       <c r="A8" s="3" t="s">
         <v>4</v>
       </c>
@@ -2200,7 +2203,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="16" customHeight="1">
       <c r="A9" s="3" t="s">
         <v>5</v>
       </c>
@@ -2214,7 +2217,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" ht="16" customHeight="1">
       <c r="A10" s="3" t="s">
         <v>22</v>
       </c>
@@ -2228,7 +2231,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" ht="16" customHeight="1">
       <c r="A11" s="3" t="s">
         <v>9</v>
       </c>
@@ -2242,7 +2245,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" ht="16" customHeight="1">
       <c r="A12" s="3" t="s">
         <v>10</v>
       </c>
@@ -2256,7 +2259,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="16" customHeight="1">
       <c r="A13" s="3" t="s">
         <v>11</v>
       </c>
@@ -2270,7 +2273,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" ht="16" customHeight="1">
       <c r="A14" s="3" t="s">
         <v>6</v>
       </c>
@@ -2284,7 +2287,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" ht="16" customHeight="1">
       <c r="A15" s="3" t="s">
         <v>7</v>
       </c>
@@ -2298,7 +2301,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="16" customHeight="1">
       <c r="A16" s="3" t="s">
         <v>21</v>
       </c>
@@ -2312,7 +2315,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="16" customHeight="1">
       <c r="A17" s="3" t="s">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
solves #747 add technical replicate
</commit_message>
<xml_diff>
--- a/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
+++ b/user-interface/src/main/resources/templates/proteomics_measurement_registration_sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kocht/SoftwareDevelopment/portlets/data-manager-app/user-interface/src/main/resources/templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DABAC10-353B-C844-9202-F385865D3A78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9AC56F-D0B2-0A41-A65E-F207BF6699C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="20500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="47">
   <si>
     <t>QBiC Sample Id*</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Injection Volume (µL)</t>
+  </si>
+  <si>
+    <t>Technical Replicate</t>
   </si>
 </sst>
 </file>
@@ -1408,7 +1411,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:Q33"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
@@ -1419,24 +1422,23 @@
     <col min="1" max="1" width="18" style="5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.6640625" style="5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.83203125" style="5" customWidth="1"/>
+    <col min="4" max="5" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="9.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.83203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11" style="5" bestFit="1" customWidth="1"/>
     <col min="18" max="16384" width="10.83203125" style="5"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16">
+    <row r="1" spans="1:17">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1447,64 +1449,68 @@
         <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16">
+    <row r="2" spans="1:17">
       <c r="A2" s="4"/>
       <c r="B2" s="4"/>
       <c r="C2" s="4"/>
       <c r="D2" s="4"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="4"/>
+      <c r="E2" s="4"/>
+      <c r="F2" s="7"/>
       <c r="G2" s="4"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="8"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
-    </row>
-    <row r="3" spans="1:16">
+      <c r="Q2" s="4"/>
+    </row>
+    <row r="3" spans="1:17">
       <c r="A3" s="4"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
@@ -1521,8 +1527,9 @@
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
-    </row>
-    <row r="4" spans="1:16">
+      <c r="Q3" s="4"/>
+    </row>
+    <row r="4" spans="1:17">
       <c r="A4" s="4"/>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
@@ -1539,8 +1546,9 @@
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
-    </row>
-    <row r="5" spans="1:16">
+      <c r="Q4" s="4"/>
+    </row>
+    <row r="5" spans="1:17">
       <c r="A5" s="4"/>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
@@ -1557,8 +1565,9 @@
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
-    </row>
-    <row r="6" spans="1:16">
+      <c r="Q5" s="4"/>
+    </row>
+    <row r="6" spans="1:17">
       <c r="A6" s="4"/>
       <c r="B6" s="4"/>
       <c r="C6" s="4"/>
@@ -1575,8 +1584,9 @@
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
       <c r="P6" s="4"/>
-    </row>
-    <row r="7" spans="1:16">
+      <c r="Q6" s="4"/>
+    </row>
+    <row r="7" spans="1:17">
       <c r="A7" s="4"/>
       <c r="B7" s="4"/>
       <c r="C7" s="4"/>
@@ -1593,8 +1603,9 @@
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
       <c r="P7" s="4"/>
-    </row>
-    <row r="8" spans="1:16">
+      <c r="Q7" s="4"/>
+    </row>
+    <row r="8" spans="1:17">
       <c r="A8" s="4"/>
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
@@ -1611,8 +1622,9 @@
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
       <c r="P8" s="4"/>
-    </row>
-    <row r="9" spans="1:16">
+      <c r="Q8" s="4"/>
+    </row>
+    <row r="9" spans="1:17">
       <c r="A9" s="4"/>
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
@@ -1629,8 +1641,9 @@
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
       <c r="P9" s="4"/>
-    </row>
-    <row r="10" spans="1:16">
+      <c r="Q9" s="4"/>
+    </row>
+    <row r="10" spans="1:17">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1647,8 +1660,9 @@
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
       <c r="P10" s="4"/>
-    </row>
-    <row r="11" spans="1:16">
+      <c r="Q10" s="4"/>
+    </row>
+    <row r="11" spans="1:17">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1665,8 +1679,9 @@
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
       <c r="P11" s="4"/>
-    </row>
-    <row r="12" spans="1:16">
+      <c r="Q11" s="4"/>
+    </row>
+    <row r="12" spans="1:17">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -1683,8 +1698,9 @@
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
       <c r="P12" s="4"/>
-    </row>
-    <row r="13" spans="1:16">
+      <c r="Q12" s="4"/>
+    </row>
+    <row r="13" spans="1:17">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -1701,8 +1717,9 @@
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
       <c r="P13" s="4"/>
-    </row>
-    <row r="14" spans="1:16">
+      <c r="Q13" s="4"/>
+    </row>
+    <row r="14" spans="1:17">
       <c r="A14" s="4"/>
       <c r="B14" s="4"/>
       <c r="C14" s="4"/>
@@ -1719,8 +1736,9 @@
       <c r="N14" s="4"/>
       <c r="O14" s="4"/>
       <c r="P14" s="4"/>
-    </row>
-    <row r="15" spans="1:16">
+      <c r="Q14" s="4"/>
+    </row>
+    <row r="15" spans="1:17">
       <c r="A15" s="4"/>
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
@@ -1737,8 +1755,9 @@
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
       <c r="P15" s="4"/>
-    </row>
-    <row r="16" spans="1:16">
+      <c r="Q15" s="4"/>
+    </row>
+    <row r="16" spans="1:17">
       <c r="A16" s="4"/>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
@@ -1749,14 +1768,15 @@
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
       <c r="J16" s="4"/>
-      <c r="K16" s="9"/>
-      <c r="L16" s="4"/>
+      <c r="K16" s="4"/>
+      <c r="L16" s="9"/>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
       <c r="P16" s="4"/>
-    </row>
-    <row r="17" spans="1:16">
+      <c r="Q16" s="4"/>
+    </row>
+    <row r="17" spans="1:17">
       <c r="A17" s="4"/>
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
@@ -1767,14 +1787,15 @@
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
       <c r="J17" s="4"/>
-      <c r="K17" s="6"/>
-      <c r="L17" s="4"/>
+      <c r="K17" s="4"/>
+      <c r="L17" s="6"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
       <c r="P17" s="4"/>
-    </row>
-    <row r="18" spans="1:16">
+      <c r="Q17" s="4"/>
+    </row>
+    <row r="18" spans="1:17">
       <c r="A18" s="4"/>
       <c r="B18" s="4"/>
       <c r="C18" s="4"/>
@@ -1785,14 +1806,15 @@
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
       <c r="J18" s="4"/>
-      <c r="K18" s="6"/>
-      <c r="L18" s="4"/>
+      <c r="K18" s="4"/>
+      <c r="L18" s="6"/>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
       <c r="P18" s="4"/>
-    </row>
-    <row r="19" spans="1:16">
+      <c r="Q18" s="4"/>
+    </row>
+    <row r="19" spans="1:17">
       <c r="A19" s="4"/>
       <c r="B19" s="4"/>
       <c r="C19" s="4"/>
@@ -1803,14 +1825,15 @@
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
-      <c r="K19" s="6"/>
-      <c r="L19" s="4"/>
+      <c r="K19" s="4"/>
+      <c r="L19" s="6"/>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
       <c r="P19" s="4"/>
-    </row>
-    <row r="20" spans="1:16">
+      <c r="Q19" s="4"/>
+    </row>
+    <row r="20" spans="1:17">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
@@ -1821,14 +1844,15 @@
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
       <c r="J20" s="4"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="4"/>
+      <c r="K20" s="4"/>
+      <c r="L20" s="6"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
       <c r="P20" s="4"/>
-    </row>
-    <row r="21" spans="1:16">
+      <c r="Q20" s="4"/>
+    </row>
+    <row r="21" spans="1:17">
       <c r="A21" s="4"/>
       <c r="B21" s="4"/>
       <c r="C21" s="4"/>
@@ -1839,14 +1863,15 @@
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
       <c r="J21" s="4"/>
-      <c r="K21" s="6"/>
-      <c r="L21" s="4"/>
+      <c r="K21" s="4"/>
+      <c r="L21" s="6"/>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
       <c r="P21" s="4"/>
-    </row>
-    <row r="22" spans="1:16">
+      <c r="Q21" s="4"/>
+    </row>
+    <row r="22" spans="1:17">
       <c r="A22" s="4"/>
       <c r="B22" s="4"/>
       <c r="C22" s="4"/>
@@ -1857,14 +1882,15 @@
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
-      <c r="K22" s="6"/>
-      <c r="L22" s="4"/>
+      <c r="K22" s="4"/>
+      <c r="L22" s="6"/>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
       <c r="P22" s="4"/>
-    </row>
-    <row r="23" spans="1:16">
+      <c r="Q22" s="4"/>
+    </row>
+    <row r="23" spans="1:17">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
@@ -1875,14 +1901,15 @@
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
       <c r="J23" s="4"/>
-      <c r="K23" s="6"/>
-      <c r="L23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="6"/>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
       <c r="P23" s="4"/>
-    </row>
-    <row r="24" spans="1:16">
+      <c r="Q23" s="4"/>
+    </row>
+    <row r="24" spans="1:17">
       <c r="A24" s="4"/>
       <c r="B24" s="4"/>
       <c r="C24" s="4"/>
@@ -1893,14 +1920,15 @@
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
       <c r="J24" s="4"/>
-      <c r="K24" s="6"/>
-      <c r="L24" s="4"/>
+      <c r="K24" s="4"/>
+      <c r="L24" s="6"/>
       <c r="M24" s="4"/>
       <c r="N24" s="4"/>
       <c r="O24" s="4"/>
       <c r="P24" s="4"/>
-    </row>
-    <row r="25" spans="1:16">
+      <c r="Q24" s="4"/>
+    </row>
+    <row r="25" spans="1:17">
       <c r="A25" s="4"/>
       <c r="B25" s="4"/>
       <c r="C25" s="4"/>
@@ -1911,14 +1939,15 @@
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
       <c r="J25" s="4"/>
-      <c r="K25" s="6"/>
-      <c r="L25" s="4"/>
+      <c r="K25" s="4"/>
+      <c r="L25" s="6"/>
       <c r="M25" s="4"/>
       <c r="N25" s="4"/>
       <c r="O25" s="4"/>
       <c r="P25" s="4"/>
-    </row>
-    <row r="26" spans="1:16">
+      <c r="Q25" s="4"/>
+    </row>
+    <row r="26" spans="1:17">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
@@ -1929,14 +1958,15 @@
       <c r="H26" s="4"/>
       <c r="I26" s="4"/>
       <c r="J26" s="4"/>
-      <c r="K26" s="6"/>
-      <c r="L26" s="4"/>
+      <c r="K26" s="4"/>
+      <c r="L26" s="6"/>
       <c r="M26" s="4"/>
       <c r="N26" s="4"/>
       <c r="O26" s="4"/>
       <c r="P26" s="4"/>
-    </row>
-    <row r="27" spans="1:16">
+      <c r="Q26" s="4"/>
+    </row>
+    <row r="27" spans="1:17">
       <c r="A27" s="4"/>
       <c r="B27" s="4"/>
       <c r="C27" s="4"/>
@@ -1947,14 +1977,15 @@
       <c r="H27" s="4"/>
       <c r="I27" s="4"/>
       <c r="J27" s="4"/>
-      <c r="K27" s="6"/>
-      <c r="L27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="6"/>
       <c r="M27" s="4"/>
       <c r="N27" s="4"/>
       <c r="O27" s="4"/>
       <c r="P27" s="4"/>
-    </row>
-    <row r="28" spans="1:16">
+      <c r="Q27" s="4"/>
+    </row>
+    <row r="28" spans="1:17">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
@@ -1965,14 +1996,15 @@
       <c r="H28" s="4"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
-      <c r="K28" s="6"/>
-      <c r="L28" s="4"/>
+      <c r="K28" s="4"/>
+      <c r="L28" s="6"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
       <c r="O28" s="4"/>
       <c r="P28" s="4"/>
-    </row>
-    <row r="29" spans="1:16">
+      <c r="Q28" s="4"/>
+    </row>
+    <row r="29" spans="1:17">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -1983,14 +2015,15 @@
       <c r="H29" s="4"/>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
-      <c r="K29" s="6"/>
-      <c r="L29" s="4"/>
+      <c r="K29" s="4"/>
+      <c r="L29" s="6"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
       <c r="P29" s="4"/>
-    </row>
-    <row r="30" spans="1:16">
+      <c r="Q29" s="4"/>
+    </row>
+    <row r="30" spans="1:17">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -2001,14 +2034,15 @@
       <c r="H30" s="4"/>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
-      <c r="K30" s="6"/>
-      <c r="L30" s="4"/>
+      <c r="K30" s="4"/>
+      <c r="L30" s="6"/>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
       <c r="P30" s="4"/>
-    </row>
-    <row r="31" spans="1:16">
+      <c r="Q30" s="4"/>
+    </row>
+    <row r="31" spans="1:17">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2019,14 +2053,15 @@
       <c r="H31" s="4"/>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="4"/>
+      <c r="K31" s="4"/>
+      <c r="L31" s="6"/>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
       <c r="P31" s="4"/>
-    </row>
-    <row r="32" spans="1:16">
+      <c r="Q31" s="4"/>
+    </row>
+    <row r="32" spans="1:17">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2037,14 +2072,15 @@
       <c r="H32" s="4"/>
       <c r="I32" s="4"/>
       <c r="J32" s="4"/>
-      <c r="K32" s="6"/>
-      <c r="L32" s="4"/>
+      <c r="K32" s="4"/>
+      <c r="L32" s="6"/>
       <c r="M32" s="4"/>
       <c r="N32" s="4"/>
       <c r="O32" s="4"/>
       <c r="P32" s="4"/>
-    </row>
-    <row r="33" spans="1:16">
+      <c r="Q32" s="4"/>
+    </row>
+    <row r="33" spans="1:17">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -2055,16 +2091,17 @@
       <c r="H33" s="4"/>
       <c r="I33" s="4"/>
       <c r="J33" s="4"/>
-      <c r="K33" s="6"/>
-      <c r="L33" s="4"/>
+      <c r="K33" s="4"/>
+      <c r="L33" s="6"/>
       <c r="M33" s="4"/>
       <c r="N33" s="4"/>
       <c r="O33" s="4"/>
       <c r="P33" s="4"/>
+      <c r="Q33" s="4"/>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="J2:J33" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="K2:K33" xr:uid="{731FEC19-6E58-BD4E-9135-3D827FA3829D}">
       <formula1>"in gel,in solution,iST proteomics kit,on beads"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>